<commit_message>
phone number of Anusch Lini corrected
</commit_message>
<xml_diff>
--- a/cfg/pubfinder_list_NLA.xlsx
+++ b/cfg/pubfinder_list_NLA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_dev\pubfinder_V2\cfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0D67EF-2BDC-46C2-A8C9-C1CE5D635006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466B6C5A-7D5D-4C08-829C-83CEC108FEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{75E81789-C525-4005-96BA-B080353C5F6C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{75E81789-C525-4005-96BA-B080353C5F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="pubfinder_list_NLA_ok" sheetId="2" r:id="rId1"/>
@@ -1979,9 +1979,6 @@
     <t>Kirchenplatz 3</t>
   </si>
   <si>
-    <t>+4991231641101</t>
-  </si>
-  <si>
     <t>reservierung@anuschlini.de</t>
   </si>
   <si>
@@ -1989,6 +1986,9 @@
   </si>
   <si>
     <t>Strasse</t>
+  </si>
+  <si>
+    <t>+4991231641126</t>
   </si>
 </sst>
 </file>
@@ -2515,34 +2515,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F2D7F2-8E23-4C59-B8E8-2949683E6C83}">
   <dimension ref="A1:W104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="39" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="81.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -2613,7 +2613,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>92</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>100</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>107</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>113</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>120</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>127</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>130</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>136</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>144</v>
       </c>
@@ -3891,7 +3891,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>150</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>157</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>638</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>170</v>
       </c>
@@ -4175,7 +4175,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>176</v>
       </c>
@@ -4246,7 +4246,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>181</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>188</v>
       </c>
@@ -4388,7 +4388,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>193</v>
       </c>
@@ -4459,7 +4459,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>199</v>
       </c>
@@ -4530,7 +4530,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>205</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>213</v>
       </c>
@@ -4672,7 +4672,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>220</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>227</v>
       </c>
@@ -4814,7 +4814,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>235</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>241</v>
       </c>
@@ -4956,7 +4956,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>248</v>
       </c>
@@ -5027,7 +5027,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>254</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>261</v>
       </c>
@@ -5169,7 +5169,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>268</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>275</v>
       </c>
@@ -5311,7 +5311,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>281</v>
       </c>
@@ -5382,7 +5382,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>287</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>293</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>299</v>
       </c>
@@ -5595,7 +5595,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>304</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>309</v>
       </c>
@@ -5737,7 +5737,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>316</v>
       </c>
@@ -5808,7 +5808,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>320</v>
       </c>
@@ -5879,7 +5879,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>324</v>
       </c>
@@ -5950,7 +5950,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>330</v>
       </c>
@@ -6021,7 +6021,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>333</v>
       </c>
@@ -6092,7 +6092,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>339</v>
       </c>
@@ -6163,7 +6163,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>343</v>
       </c>
@@ -6234,7 +6234,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>349</v>
       </c>
@@ -6305,7 +6305,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>352</v>
       </c>
@@ -6376,7 +6376,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>356</v>
       </c>
@@ -6447,7 +6447,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>363</v>
       </c>
@@ -6518,7 +6518,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>370</v>
       </c>
@@ -6589,7 +6589,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>631</v>
       </c>
@@ -6657,7 +6657,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>376</v>
       </c>
@@ -6728,7 +6728,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>382</v>
       </c>
@@ -6799,7 +6799,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>389</v>
       </c>
@@ -6870,7 +6870,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>395</v>
       </c>
@@ -6941,7 +6941,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>402</v>
       </c>
@@ -7012,7 +7012,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>406</v>
       </c>
@@ -7083,7 +7083,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>410</v>
       </c>
@@ -7154,7 +7154,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>416</v>
       </c>
@@ -7225,7 +7225,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>640</v>
       </c>
@@ -7242,13 +7242,13 @@
         <v>418</v>
       </c>
       <c r="F67" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="G67" s="4" t="s">
         <v>643</v>
       </c>
-      <c r="G67" s="4" t="s">
+      <c r="H67" s="4" t="s">
         <v>644</v>
-      </c>
-      <c r="H67" s="4" t="s">
-        <v>645</v>
       </c>
       <c r="I67" t="s">
         <v>29</v>
@@ -7296,7 +7296,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>422</v>
       </c>
@@ -7367,7 +7367,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>427</v>
       </c>
@@ -7438,7 +7438,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>434</v>
       </c>
@@ -7509,7 +7509,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>439</v>
       </c>
@@ -7580,7 +7580,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>443</v>
       </c>
@@ -7651,7 +7651,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>447</v>
       </c>
@@ -7722,7 +7722,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>453</v>
       </c>
@@ -7793,7 +7793,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>458</v>
       </c>
@@ -7864,7 +7864,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>463</v>
       </c>
@@ -7935,7 +7935,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>470</v>
       </c>
@@ -8006,7 +8006,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>473</v>
       </c>
@@ -8077,7 +8077,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>476</v>
       </c>
@@ -8148,7 +8148,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>480</v>
       </c>
@@ -8219,7 +8219,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>486</v>
       </c>
@@ -8290,7 +8290,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>491</v>
       </c>
@@ -8361,7 +8361,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>498</v>
       </c>
@@ -8432,7 +8432,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>504</v>
       </c>
@@ -8503,7 +8503,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>511</v>
       </c>
@@ -8574,7 +8574,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>517</v>
       </c>
@@ -8645,7 +8645,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>525</v>
       </c>
@@ -8716,7 +8716,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>531</v>
       </c>
@@ -8787,7 +8787,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>536</v>
       </c>
@@ -8858,7 +8858,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>542</v>
       </c>
@@ -8929,7 +8929,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>548</v>
       </c>
@@ -9000,7 +9000,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>554</v>
       </c>
@@ -9071,7 +9071,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>561</v>
       </c>
@@ -9142,7 +9142,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>566</v>
       </c>
@@ -9213,7 +9213,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>570</v>
       </c>
@@ -9284,7 +9284,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>576</v>
       </c>
@@ -9355,7 +9355,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>580</v>
       </c>
@@ -9426,7 +9426,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>587</v>
       </c>
@@ -9497,7 +9497,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>596</v>
       </c>
@@ -9568,7 +9568,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>601</v>
       </c>
@@ -9639,7 +9639,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>607</v>
       </c>
@@ -9710,7 +9710,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>613</v>
       </c>
@@ -9781,7 +9781,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>618</v>
       </c>
@@ -9852,7 +9852,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>624</v>
       </c>
@@ -9944,7 +9944,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Zu den Linden Utzmannsbach added
</commit_message>
<xml_diff>
--- a/cfg/pubfinder_list_NLA.xlsx
+++ b/cfg/pubfinder_list_NLA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_dev\pubfinder_V2\cfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466B6C5A-7D5D-4C08-829C-83CEC108FEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB3BE44-7B57-40D6-B041-782012B3A84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{75E81789-C525-4005-96BA-B080353C5F6C}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">pubfinder_list_NLA_ok!$A$1:$W$104</definedName>
+    <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">pubfinder_list_NLA_ok!$A$1:$W$105</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2288" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2310" uniqueCount="653">
   <si>
     <t>Name</t>
   </si>
@@ -1989,6 +1989,24 @@
   </si>
   <si>
     <t>+4991231641126</t>
+  </si>
+  <si>
+    <t>Zu den Linden</t>
+  </si>
+  <si>
+    <t>Utzmannsbach 11</t>
+  </si>
+  <si>
+    <t>+499155 446</t>
+  </si>
+  <si>
+    <t>https://www.gasthaus-zu-den-linden.de/</t>
+  </si>
+  <si>
+    <t>info@gasthaus-zu-den-linden.de</t>
+  </si>
+  <si>
+    <t>10:00 - 15:00</t>
   </si>
 </sst>
 </file>
@@ -2165,8 +2183,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C4BF8B3-CB62-48F7-AAC2-6E12CB367C86}" name="pubfinder_list_NLA_ok" displayName="pubfinder_list_NLA_ok" ref="A1:W104" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:W104" xr:uid="{1C4BF8B3-CB62-48F7-AAC2-6E12CB367C86}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C4BF8B3-CB62-48F7-AAC2-6E12CB367C86}" name="pubfinder_list_NLA_ok" displayName="pubfinder_list_NLA_ok" ref="A1:W105" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:W105" xr:uid="{1C4BF8B3-CB62-48F7-AAC2-6E12CB367C86}"/>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{92103B2C-FCC3-42D2-95DB-A3F77D77EC29}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="21"/>
     <tableColumn id="2" xr3:uid="{86208C35-2046-4F53-B583-F5FD55ED84C8}" uniqueName="2" name="Typ" queryTableFieldId="2" dataDxfId="20"/>
@@ -2513,10 +2531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F2D7F2-8E23-4C59-B8E8-2949683E6C83}">
-  <dimension ref="A1:W104"/>
+  <dimension ref="A1:W105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="M70" workbookViewId="0">
+      <selection activeCell="V100" sqref="V100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9570,28 +9588,28 @@
     </row>
     <row r="100" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>601</v>
+        <v>647</v>
       </c>
       <c r="B100" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="C100" t="s">
-        <v>602</v>
+        <v>648</v>
       </c>
       <c r="D100">
-        <v>91247</v>
+        <v>91245</v>
       </c>
       <c r="E100" t="s">
-        <v>603</v>
-      </c>
-      <c r="F100" t="s">
-        <v>604</v>
-      </c>
-      <c r="G100" t="s">
-        <v>27</v>
-      </c>
-      <c r="H100" t="s">
-        <v>605</v>
+        <v>589</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="G100" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="H100" s="4" t="s">
+        <v>650</v>
       </c>
       <c r="I100" t="s">
         <v>29</v>
@@ -9600,13 +9618,13 @@
         <v>29</v>
       </c>
       <c r="K100" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L100" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="M100" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="N100" t="s">
         <v>30</v>
@@ -9621,19 +9639,19 @@
         <v>29</v>
       </c>
       <c r="R100" t="s">
-        <v>29</v>
+        <v>652</v>
       </c>
       <c r="S100" t="s">
-        <v>29</v>
+        <v>586</v>
       </c>
       <c r="T100" t="s">
-        <v>29</v>
+        <v>586</v>
       </c>
       <c r="U100" t="s">
-        <v>72</v>
+        <v>586</v>
       </c>
       <c r="V100" t="s">
-        <v>606</v>
+        <v>586</v>
       </c>
       <c r="W100" t="s">
         <v>27</v>
@@ -9641,13 +9659,13 @@
     </row>
     <row r="101" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="B101" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C101" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="D101">
         <v>91247</v>
@@ -9656,28 +9674,28 @@
         <v>603</v>
       </c>
       <c r="F101" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="G101" t="s">
-        <v>610</v>
+        <v>27</v>
       </c>
       <c r="H101" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="I101" t="s">
         <v>29</v>
       </c>
       <c r="J101" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K101" t="s">
         <v>29</v>
       </c>
       <c r="L101" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="M101" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="N101" t="s">
         <v>30</v>
@@ -9689,22 +9707,22 @@
         <v>29</v>
       </c>
       <c r="Q101" t="s">
-        <v>612</v>
+        <v>29</v>
       </c>
       <c r="R101" t="s">
         <v>29</v>
       </c>
       <c r="S101" t="s">
-        <v>612</v>
+        <v>29</v>
       </c>
       <c r="T101" t="s">
-        <v>612</v>
+        <v>29</v>
       </c>
       <c r="U101" t="s">
-        <v>612</v>
+        <v>72</v>
       </c>
       <c r="V101" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="W101" t="s">
         <v>27</v>
@@ -9712,13 +9730,13 @@
     </row>
     <row r="102" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="B102" t="s">
         <v>23</v>
       </c>
       <c r="C102" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="D102">
         <v>91247</v>
@@ -9727,25 +9745,25 @@
         <v>603</v>
       </c>
       <c r="F102" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="G102" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="H102" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="I102" t="s">
         <v>29</v>
       </c>
       <c r="J102" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K102" t="s">
         <v>29</v>
       </c>
       <c r="L102" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="M102" t="s">
         <v>41</v>
@@ -9760,22 +9778,22 @@
         <v>29</v>
       </c>
       <c r="Q102" t="s">
-        <v>29</v>
+        <v>612</v>
       </c>
       <c r="R102" t="s">
         <v>29</v>
       </c>
       <c r="S102" t="s">
-        <v>29</v>
+        <v>612</v>
       </c>
       <c r="T102" t="s">
-        <v>469</v>
+        <v>612</v>
       </c>
       <c r="U102" t="s">
-        <v>469</v>
+        <v>612</v>
       </c>
       <c r="V102" t="s">
-        <v>57</v>
+        <v>612</v>
       </c>
       <c r="W102" t="s">
         <v>27</v>
@@ -9783,28 +9801,28 @@
     </row>
     <row r="103" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="B103" t="s">
         <v>23</v>
       </c>
       <c r="C103" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="D103">
-        <v>91367</v>
+        <v>91247</v>
       </c>
       <c r="E103" t="s">
-        <v>620</v>
+        <v>603</v>
       </c>
       <c r="F103" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="G103" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="H103" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="I103" t="s">
         <v>29</v>
@@ -9816,7 +9834,7 @@
         <v>29</v>
       </c>
       <c r="L103" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="M103" t="s">
         <v>41</v>
@@ -9837,16 +9855,16 @@
         <v>29</v>
       </c>
       <c r="S103" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="T103" t="s">
-        <v>72</v>
+        <v>469</v>
       </c>
       <c r="U103" t="s">
-        <v>72</v>
+        <v>469</v>
       </c>
       <c r="V103" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="W103" t="s">
         <v>27</v>
@@ -9854,13 +9872,13 @@
     </row>
     <row r="104" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="B104" t="s">
         <v>23</v>
       </c>
       <c r="C104" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="D104">
         <v>91367</v>
@@ -9869,22 +9887,22 @@
         <v>620</v>
       </c>
       <c r="F104" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="G104" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="H104" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="I104" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J104" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K104" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L104" t="s">
         <v>40</v>
@@ -9896,30 +9914,101 @@
         <v>30</v>
       </c>
       <c r="O104" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P104" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>29</v>
+      </c>
+      <c r="R104" t="s">
+        <v>29</v>
+      </c>
+      <c r="S104" t="s">
+        <v>71</v>
+      </c>
+      <c r="T104" t="s">
+        <v>72</v>
+      </c>
+      <c r="U104" t="s">
+        <v>72</v>
+      </c>
+      <c r="V104" t="s">
+        <v>72</v>
+      </c>
+      <c r="W104" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="105" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>624</v>
+      </c>
+      <c r="B105" t="s">
+        <v>23</v>
+      </c>
+      <c r="C105" t="s">
+        <v>625</v>
+      </c>
+      <c r="D105">
+        <v>91367</v>
+      </c>
+      <c r="E105" t="s">
+        <v>620</v>
+      </c>
+      <c r="F105" t="s">
+        <v>626</v>
+      </c>
+      <c r="G105" t="s">
+        <v>627</v>
+      </c>
+      <c r="H105" t="s">
+        <v>628</v>
+      </c>
+      <c r="I105" t="s">
+        <v>38</v>
+      </c>
+      <c r="J105" t="s">
+        <v>39</v>
+      </c>
+      <c r="K105" t="s">
+        <v>47</v>
+      </c>
+      <c r="L105" t="s">
+        <v>40</v>
+      </c>
+      <c r="M105" t="s">
+        <v>41</v>
+      </c>
+      <c r="N105" t="s">
+        <v>30</v>
+      </c>
+      <c r="O105" t="s">
+        <v>29</v>
+      </c>
+      <c r="P105" t="s">
         <v>629</v>
       </c>
-      <c r="Q104" t="s">
+      <c r="Q105" t="s">
         <v>629</v>
       </c>
-      <c r="R104" t="s">
+      <c r="R105" t="s">
         <v>629</v>
       </c>
-      <c r="S104" t="s">
+      <c r="S105" t="s">
         <v>629</v>
       </c>
-      <c r="T104" t="s">
+      <c r="T105" t="s">
         <v>629</v>
       </c>
-      <c r="U104" t="s">
+      <c r="U105" t="s">
         <v>630</v>
       </c>
-      <c r="V104" t="s">
-        <v>29</v>
-      </c>
-      <c r="W104" t="s">
+      <c r="V105" t="s">
+        <v>29</v>
+      </c>
+      <c r="W105" t="s">
         <v>27</v>
       </c>
     </row>
@@ -9930,10 +10019,12 @@
     <hyperlink ref="H79" r:id="rId3" xr:uid="{AD9CFEB0-515E-47DE-A619-8A0566327566}"/>
     <hyperlink ref="G67" r:id="rId4" xr:uid="{C5402745-E279-4144-A7EA-01FCE7A4E404}"/>
     <hyperlink ref="H67" r:id="rId5" xr:uid="{679F818E-03B4-4BF2-B47A-7E4540C537AF}"/>
+    <hyperlink ref="H100" r:id="rId6" xr:uid="{64B05FEF-865E-4E04-B288-9B0F0E91EB19}"/>
+    <hyperlink ref="G100" r:id="rId7" xr:uid="{1C619C93-40F6-455D-B3C4-D8F5DA0E79E2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Afroditi greek pub in Lauf added
</commit_message>
<xml_diff>
--- a/cfg/pubfinder_list_NLA.xlsx
+++ b/cfg/pubfinder_list_NLA.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_dev\pubfinder_V2\cfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB3BE44-7B57-40D6-B041-782012B3A84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D727DF-A89C-4F54-9774-108CF2255C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{75E81789-C525-4005-96BA-B080353C5F6C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{75E81789-C525-4005-96BA-B080353C5F6C}"/>
   </bookViews>
   <sheets>
-    <sheet name="pubfinder_list_NLA_ok" sheetId="2" r:id="rId1"/>
+    <sheet name="pubfinder_list_NLA" sheetId="2" r:id="rId1"/>
     <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">pubfinder_list_NLA_ok!$A$1:$W$105</definedName>
+    <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">pubfinder_list_NLA!$A$1:$W$106</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2310" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2332" uniqueCount="658">
   <si>
     <t>Name</t>
   </si>
@@ -2007,6 +2007,21 @@
   </si>
   <si>
     <t>10:00 - 15:00</t>
+  </si>
+  <si>
+    <t>Afroditi</t>
+  </si>
+  <si>
+    <t>Samstagstr. 20</t>
+  </si>
+  <si>
+    <t>+4991239892860</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php/?id=100061930315399</t>
+  </si>
+  <si>
+    <t>11:00 - 14:00 &amp; 17:00 - 21:00</t>
   </si>
 </sst>
 </file>
@@ -2183,8 +2198,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C4BF8B3-CB62-48F7-AAC2-6E12CB367C86}" name="pubfinder_list_NLA_ok" displayName="pubfinder_list_NLA_ok" ref="A1:W105" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:W105" xr:uid="{1C4BF8B3-CB62-48F7-AAC2-6E12CB367C86}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C4BF8B3-CB62-48F7-AAC2-6E12CB367C86}" name="pubfinder_list_NLA_ok" displayName="pubfinder_list_NLA_ok" ref="A1:W106" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:W106" xr:uid="{1C4BF8B3-CB62-48F7-AAC2-6E12CB367C86}"/>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{92103B2C-FCC3-42D2-95DB-A3F77D77EC29}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="21"/>
     <tableColumn id="2" xr3:uid="{86208C35-2046-4F53-B583-F5FD55ED84C8}" uniqueName="2" name="Typ" queryTableFieldId="2" dataDxfId="20"/>
@@ -2531,36 +2546,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F2D7F2-8E23-4C59-B8E8-2949683E6C83}">
-  <dimension ref="A1:W105"/>
+  <dimension ref="A1:W106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M70" workbookViewId="0">
-      <selection activeCell="V100" sqref="V100"/>
+    <sheetView tabSelected="1" topLeftCell="Q61" workbookViewId="0">
+      <selection activeCell="Y86" sqref="Y86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="39" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="81.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="25.26953125" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2631,7 +2646,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -2702,7 +2717,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -2773,7 +2788,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -2844,7 +2859,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2915,7 +2930,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -2986,7 +3001,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -3057,7 +3072,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -3128,7 +3143,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -3199,7 +3214,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -3270,7 +3285,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>92</v>
       </c>
@@ -3341,7 +3356,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>100</v>
       </c>
@@ -3412,7 +3427,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>107</v>
       </c>
@@ -3483,7 +3498,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>113</v>
       </c>
@@ -3554,7 +3569,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>120</v>
       </c>
@@ -3625,7 +3640,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>127</v>
       </c>
@@ -3696,7 +3711,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>130</v>
       </c>
@@ -3767,7 +3782,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>136</v>
       </c>
@@ -3838,7 +3853,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>144</v>
       </c>
@@ -3909,7 +3924,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>150</v>
       </c>
@@ -3980,7 +3995,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>157</v>
       </c>
@@ -4051,7 +4066,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>638</v>
       </c>
@@ -4122,7 +4137,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>170</v>
       </c>
@@ -4193,7 +4208,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>176</v>
       </c>
@@ -4264,7 +4279,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>181</v>
       </c>
@@ -4335,7 +4350,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>188</v>
       </c>
@@ -4406,7 +4421,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>193</v>
       </c>
@@ -4477,7 +4492,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>199</v>
       </c>
@@ -4548,7 +4563,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>205</v>
       </c>
@@ -4619,7 +4634,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>213</v>
       </c>
@@ -4690,7 +4705,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>220</v>
       </c>
@@ -4761,7 +4776,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>227</v>
       </c>
@@ -4832,7 +4847,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>235</v>
       </c>
@@ -4903,7 +4918,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>241</v>
       </c>
@@ -4974,7 +4989,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>248</v>
       </c>
@@ -5045,7 +5060,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>254</v>
       </c>
@@ -5116,7 +5131,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>261</v>
       </c>
@@ -5187,7 +5202,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>268</v>
       </c>
@@ -5258,7 +5273,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>275</v>
       </c>
@@ -5329,7 +5344,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>281</v>
       </c>
@@ -5400,7 +5415,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>287</v>
       </c>
@@ -5471,7 +5486,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>293</v>
       </c>
@@ -5542,7 +5557,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>299</v>
       </c>
@@ -5613,7 +5628,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>304</v>
       </c>
@@ -5684,7 +5699,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>309</v>
       </c>
@@ -5755,7 +5770,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>316</v>
       </c>
@@ -5826,7 +5841,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>320</v>
       </c>
@@ -5897,7 +5912,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>324</v>
       </c>
@@ -5968,7 +5983,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>330</v>
       </c>
@@ -6039,7 +6054,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>333</v>
       </c>
@@ -6110,7 +6125,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>339</v>
       </c>
@@ -6181,7 +6196,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>343</v>
       </c>
@@ -6252,7 +6267,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>349</v>
       </c>
@@ -6323,7 +6338,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>352</v>
       </c>
@@ -6394,7 +6409,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>356</v>
       </c>
@@ -6465,7 +6480,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>363</v>
       </c>
@@ -6536,7 +6551,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>370</v>
       </c>
@@ -6607,7 +6622,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>631</v>
       </c>
@@ -6675,7 +6690,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>376</v>
       </c>
@@ -6746,7 +6761,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>382</v>
       </c>
@@ -6817,7 +6832,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>389</v>
       </c>
@@ -6888,7 +6903,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>395</v>
       </c>
@@ -6959,7 +6974,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>402</v>
       </c>
@@ -7030,7 +7045,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>406</v>
       </c>
@@ -7101,7 +7116,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>410</v>
       </c>
@@ -7172,15 +7187,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>416</v>
+        <v>653</v>
       </c>
       <c r="B66" t="s">
-        <v>93</v>
+        <v>249</v>
       </c>
       <c r="C66" t="s">
-        <v>417</v>
+        <v>654</v>
       </c>
       <c r="D66">
         <v>91207</v>
@@ -7188,17 +7203,17 @@
       <c r="E66" t="s">
         <v>418</v>
       </c>
-      <c r="F66" t="s">
-        <v>419</v>
+      <c r="F66" s="2" t="s">
+        <v>655</v>
       </c>
       <c r="G66" t="s">
         <v>27</v>
       </c>
-      <c r="H66" t="s">
-        <v>420</v>
+      <c r="H66" s="4" t="s">
+        <v>656</v>
       </c>
       <c r="I66" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J66" t="s">
         <v>39</v>
@@ -7219,39 +7234,39 @@
         <v>29</v>
       </c>
       <c r="P66" t="s">
-        <v>421</v>
+        <v>29</v>
       </c>
       <c r="Q66" t="s">
-        <v>421</v>
+        <v>56</v>
       </c>
       <c r="R66" t="s">
-        <v>421</v>
+        <v>56</v>
       </c>
       <c r="S66" t="s">
-        <v>421</v>
+        <v>56</v>
       </c>
       <c r="T66" t="s">
-        <v>421</v>
+        <v>56</v>
       </c>
       <c r="U66" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="V66" t="s">
-        <v>29</v>
+        <v>657</v>
       </c>
       <c r="W66" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>640</v>
+        <v>416</v>
       </c>
       <c r="B67" t="s">
-        <v>641</v>
+        <v>93</v>
       </c>
       <c r="C67" t="s">
-        <v>642</v>
+        <v>417</v>
       </c>
       <c r="D67">
         <v>91207</v>
@@ -7259,17 +7274,17 @@
       <c r="E67" t="s">
         <v>418</v>
       </c>
-      <c r="F67" s="2" t="s">
-        <v>646</v>
-      </c>
-      <c r="G67" s="4" t="s">
-        <v>643</v>
-      </c>
-      <c r="H67" s="4" t="s">
-        <v>644</v>
+      <c r="F67" t="s">
+        <v>419</v>
+      </c>
+      <c r="G67" t="s">
+        <v>27</v>
+      </c>
+      <c r="H67" t="s">
+        <v>420</v>
       </c>
       <c r="I67" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="J67" t="s">
         <v>39</v>
@@ -7284,45 +7299,45 @@
         <v>41</v>
       </c>
       <c r="N67" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O67" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="P67" t="s">
-        <v>29</v>
+        <v>421</v>
       </c>
       <c r="Q67" t="s">
-        <v>452</v>
+        <v>421</v>
       </c>
       <c r="R67" t="s">
-        <v>452</v>
+        <v>421</v>
       </c>
       <c r="S67" t="s">
-        <v>452</v>
+        <v>421</v>
       </c>
       <c r="T67" t="s">
-        <v>452</v>
+        <v>421</v>
       </c>
       <c r="U67" t="s">
-        <v>452</v>
+        <v>29</v>
       </c>
       <c r="V67" t="s">
-        <v>452</v>
+        <v>29</v>
       </c>
       <c r="W67" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>422</v>
+        <v>640</v>
       </c>
       <c r="B68" t="s">
-        <v>51</v>
+        <v>641</v>
       </c>
       <c r="C68" t="s">
-        <v>423</v>
+        <v>642</v>
       </c>
       <c r="D68">
         <v>91207</v>
@@ -7330,23 +7345,23 @@
       <c r="E68" t="s">
         <v>418</v>
       </c>
-      <c r="F68" t="s">
-        <v>424</v>
-      </c>
-      <c r="G68" t="s">
-        <v>27</v>
-      </c>
-      <c r="H68" t="s">
-        <v>425</v>
+      <c r="F68" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>643</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>644</v>
       </c>
       <c r="I68" t="s">
         <v>29</v>
       </c>
       <c r="J68" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K68" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L68" t="s">
         <v>40</v>
@@ -7364,36 +7379,36 @@
         <v>29</v>
       </c>
       <c r="Q68" t="s">
-        <v>29</v>
+        <v>452</v>
       </c>
       <c r="R68" t="s">
-        <v>29</v>
+        <v>452</v>
       </c>
       <c r="S68" t="s">
-        <v>426</v>
+        <v>452</v>
       </c>
       <c r="T68" t="s">
-        <v>426</v>
+        <v>452</v>
       </c>
       <c r="U68" t="s">
-        <v>426</v>
+        <v>452</v>
       </c>
       <c r="V68" t="s">
-        <v>426</v>
+        <v>452</v>
       </c>
       <c r="W68" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="B69" t="s">
-        <v>249</v>
+        <v>51</v>
       </c>
       <c r="C69" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D69">
         <v>91207</v>
@@ -7402,13 +7417,13 @@
         <v>418</v>
       </c>
       <c r="F69" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="G69" t="s">
-        <v>430</v>
+        <v>27</v>
       </c>
       <c r="H69" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="I69" t="s">
         <v>29</v>
@@ -7417,7 +7432,7 @@
         <v>29</v>
       </c>
       <c r="K69" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L69" t="s">
         <v>40</v>
@@ -7438,33 +7453,33 @@
         <v>29</v>
       </c>
       <c r="R69" t="s">
-        <v>432</v>
+        <v>29</v>
       </c>
       <c r="S69" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="T69" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="U69" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="V69" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="W69" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="B70" t="s">
-        <v>23</v>
+        <v>249</v>
       </c>
       <c r="C70" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="D70">
         <v>91207</v>
@@ -7473,13 +7488,13 @@
         <v>418</v>
       </c>
       <c r="F70" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="G70" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="H70" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="I70" t="s">
         <v>29</v>
@@ -7488,10 +7503,10 @@
         <v>29</v>
       </c>
       <c r="K70" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L70" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="M70" t="s">
         <v>41</v>
@@ -7509,33 +7524,33 @@
         <v>29</v>
       </c>
       <c r="R70" t="s">
-        <v>29</v>
+        <v>432</v>
       </c>
       <c r="S70" t="s">
-        <v>29</v>
+        <v>433</v>
       </c>
       <c r="T70" t="s">
-        <v>71</v>
+        <v>432</v>
       </c>
       <c r="U70" t="s">
-        <v>329</v>
+        <v>432</v>
       </c>
       <c r="V70" t="s">
-        <v>329</v>
+        <v>432</v>
       </c>
       <c r="W70" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B71" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="C71" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="D71">
         <v>91207</v>
@@ -7544,25 +7559,25 @@
         <v>418</v>
       </c>
       <c r="F71" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="G71" t="s">
-        <v>27</v>
+        <v>437</v>
       </c>
       <c r="H71" t="s">
-        <v>27</v>
+        <v>438</v>
       </c>
       <c r="I71" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J71" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K71" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L71" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="M71" t="s">
         <v>41</v>
@@ -7574,39 +7589,39 @@
         <v>31</v>
       </c>
       <c r="P71" t="s">
-        <v>292</v>
+        <v>29</v>
       </c>
       <c r="Q71" t="s">
-        <v>292</v>
+        <v>29</v>
       </c>
       <c r="R71" t="s">
-        <v>292</v>
+        <v>29</v>
       </c>
       <c r="S71" t="s">
-        <v>292</v>
+        <v>29</v>
       </c>
       <c r="T71" t="s">
-        <v>292</v>
+        <v>71</v>
       </c>
       <c r="U71" t="s">
-        <v>292</v>
+        <v>329</v>
       </c>
       <c r="V71" t="s">
-        <v>442</v>
+        <v>329</v>
       </c>
       <c r="W71" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B72" t="s">
         <v>66</v>
       </c>
       <c r="C72" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="D72">
         <v>91207</v>
@@ -7615,16 +7630,16 @@
         <v>418</v>
       </c>
       <c r="F72" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="G72" t="s">
         <v>27</v>
       </c>
       <c r="H72" t="s">
-        <v>446</v>
+        <v>27</v>
       </c>
       <c r="I72" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="J72" t="s">
         <v>39</v>
@@ -7642,42 +7657,42 @@
         <v>30</v>
       </c>
       <c r="O72" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P72" t="s">
-        <v>29</v>
+        <v>292</v>
       </c>
       <c r="Q72" t="s">
-        <v>232</v>
+        <v>292</v>
       </c>
       <c r="R72" t="s">
-        <v>232</v>
+        <v>292</v>
       </c>
       <c r="S72" t="s">
-        <v>232</v>
+        <v>292</v>
       </c>
       <c r="T72" t="s">
-        <v>232</v>
+        <v>292</v>
       </c>
       <c r="U72" t="s">
-        <v>253</v>
+        <v>292</v>
       </c>
       <c r="V72" t="s">
-        <v>29</v>
+        <v>442</v>
       </c>
       <c r="W72" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B73" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C73" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D73">
         <v>91207</v>
@@ -7686,19 +7701,19 @@
         <v>418</v>
       </c>
       <c r="F73" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="G73" t="s">
-        <v>450</v>
+        <v>27</v>
       </c>
       <c r="H73" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="I73" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J73" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K73" t="s">
         <v>47</v>
@@ -7713,42 +7728,42 @@
         <v>30</v>
       </c>
       <c r="O73" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="P73" t="s">
-        <v>452</v>
+        <v>29</v>
       </c>
       <c r="Q73" t="s">
-        <v>29</v>
+        <v>232</v>
       </c>
       <c r="R73" t="s">
-        <v>452</v>
+        <v>232</v>
       </c>
       <c r="S73" t="s">
-        <v>452</v>
+        <v>232</v>
       </c>
       <c r="T73" t="s">
-        <v>452</v>
+        <v>232</v>
       </c>
       <c r="U73" t="s">
-        <v>292</v>
+        <v>253</v>
       </c>
       <c r="V73" t="s">
-        <v>292</v>
+        <v>29</v>
       </c>
       <c r="W73" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="B74" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C74" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="D74">
         <v>91207</v>
@@ -7757,16 +7772,16 @@
         <v>418</v>
       </c>
       <c r="F74" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="G74" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="H74" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="I74" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="J74" t="s">
         <v>29</v>
@@ -7787,39 +7802,39 @@
         <v>31</v>
       </c>
       <c r="P74" t="s">
-        <v>29</v>
+        <v>452</v>
       </c>
       <c r="Q74" t="s">
         <v>29</v>
       </c>
       <c r="R74" t="s">
-        <v>106</v>
+        <v>452</v>
       </c>
       <c r="S74" t="s">
-        <v>106</v>
+        <v>452</v>
       </c>
       <c r="T74" t="s">
-        <v>106</v>
+        <v>452</v>
       </c>
       <c r="U74" t="s">
-        <v>106</v>
+        <v>292</v>
       </c>
       <c r="V74" t="s">
-        <v>106</v>
+        <v>292</v>
       </c>
       <c r="W74" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="B75" t="s">
         <v>23</v>
       </c>
       <c r="C75" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="D75">
         <v>91207</v>
@@ -7828,13 +7843,13 @@
         <v>418</v>
       </c>
       <c r="F75" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="G75" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="H75" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="I75" t="s">
         <v>29</v>
@@ -7864,33 +7879,33 @@
         <v>29</v>
       </c>
       <c r="R75" t="s">
-        <v>369</v>
+        <v>106</v>
       </c>
       <c r="S75" t="s">
-        <v>369</v>
+        <v>106</v>
       </c>
       <c r="T75" t="s">
-        <v>369</v>
+        <v>106</v>
       </c>
       <c r="U75" t="s">
-        <v>369</v>
+        <v>106</v>
       </c>
       <c r="V75" t="s">
-        <v>369</v>
+        <v>106</v>
       </c>
       <c r="W75" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="B76" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="C76" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="D76">
         <v>91207</v>
@@ -7899,19 +7914,19 @@
         <v>418</v>
       </c>
       <c r="F76" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="G76" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="H76" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="I76" t="s">
         <v>29</v>
       </c>
       <c r="J76" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K76" t="s">
         <v>47</v>
@@ -7932,36 +7947,36 @@
         <v>29</v>
       </c>
       <c r="Q76" t="s">
-        <v>468</v>
+        <v>29</v>
       </c>
       <c r="R76" t="s">
-        <v>469</v>
+        <v>369</v>
       </c>
       <c r="S76" t="s">
-        <v>469</v>
+        <v>369</v>
       </c>
       <c r="T76" t="s">
-        <v>469</v>
+        <v>369</v>
       </c>
       <c r="U76" t="s">
-        <v>469</v>
+        <v>369</v>
       </c>
       <c r="V76" t="s">
-        <v>469</v>
+        <v>369</v>
       </c>
       <c r="W76" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="B77" t="s">
         <v>66</v>
       </c>
       <c r="C77" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="D77">
         <v>91207</v>
@@ -7970,13 +7985,13 @@
         <v>418</v>
       </c>
       <c r="F77" t="s">
-        <v>445</v>
+        <v>465</v>
       </c>
       <c r="G77" t="s">
-        <v>27</v>
+        <v>466</v>
       </c>
       <c r="H77" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="I77" t="s">
         <v>29</v>
@@ -7997,42 +8012,42 @@
         <v>30</v>
       </c>
       <c r="O77" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P77" t="s">
         <v>29</v>
       </c>
       <c r="Q77" t="s">
-        <v>232</v>
+        <v>468</v>
       </c>
       <c r="R77" t="s">
-        <v>232</v>
+        <v>469</v>
       </c>
       <c r="S77" t="s">
-        <v>232</v>
+        <v>469</v>
       </c>
       <c r="T77" t="s">
-        <v>232</v>
+        <v>469</v>
       </c>
       <c r="U77" t="s">
-        <v>253</v>
+        <v>469</v>
       </c>
       <c r="V77" t="s">
-        <v>29</v>
+        <v>469</v>
       </c>
       <c r="W77" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B78" t="s">
         <v>66</v>
       </c>
       <c r="C78" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D78">
         <v>91207</v>
@@ -8047,7 +8062,7 @@
         <v>27</v>
       </c>
       <c r="H78" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="I78" t="s">
         <v>29</v>
@@ -8068,42 +8083,42 @@
         <v>30</v>
       </c>
       <c r="O78" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="P78" t="s">
         <v>29</v>
       </c>
       <c r="Q78" t="s">
-        <v>292</v>
+        <v>232</v>
       </c>
       <c r="R78" t="s">
-        <v>292</v>
+        <v>232</v>
       </c>
       <c r="S78" t="s">
-        <v>292</v>
+        <v>232</v>
       </c>
       <c r="T78" t="s">
-        <v>292</v>
+        <v>232</v>
       </c>
       <c r="U78" t="s">
-        <v>292</v>
+        <v>253</v>
       </c>
       <c r="V78" t="s">
-        <v>292</v>
+        <v>29</v>
       </c>
       <c r="W78" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B79" t="s">
         <v>66</v>
       </c>
       <c r="C79" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="D79">
         <v>91207</v>
@@ -8112,22 +8127,22 @@
         <v>418</v>
       </c>
       <c r="F79" t="s">
-        <v>478</v>
+        <v>445</v>
       </c>
       <c r="G79" t="s">
         <v>27</v>
       </c>
-      <c r="H79" s="4" t="s">
-        <v>639</v>
+      <c r="H79" t="s">
+        <v>475</v>
       </c>
       <c r="I79" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J79" t="s">
         <v>39</v>
       </c>
       <c r="K79" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L79" t="s">
         <v>40</v>
@@ -8142,39 +8157,39 @@
         <v>31</v>
       </c>
       <c r="P79" t="s">
-        <v>479</v>
+        <v>29</v>
       </c>
       <c r="Q79" t="s">
-        <v>479</v>
+        <v>292</v>
       </c>
       <c r="R79" t="s">
-        <v>29</v>
+        <v>292</v>
       </c>
       <c r="S79" t="s">
-        <v>479</v>
+        <v>292</v>
       </c>
       <c r="T79" t="s">
-        <v>479</v>
+        <v>292</v>
       </c>
       <c r="U79" t="s">
-        <v>479</v>
+        <v>292</v>
       </c>
       <c r="V79" t="s">
-        <v>479</v>
+        <v>292</v>
       </c>
       <c r="W79" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B80" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="C80" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="D80">
         <v>91207</v>
@@ -8183,13 +8198,13 @@
         <v>418</v>
       </c>
       <c r="F80" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="G80" t="s">
-        <v>483</v>
-      </c>
-      <c r="H80" t="s">
-        <v>484</v>
+        <v>27</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>639</v>
       </c>
       <c r="I80" t="s">
         <v>38</v>
@@ -8198,7 +8213,7 @@
         <v>39</v>
       </c>
       <c r="K80" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L80" t="s">
         <v>40</v>
@@ -8210,42 +8225,42 @@
         <v>30</v>
       </c>
       <c r="O80" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P80" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="Q80" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="R80" t="s">
-        <v>485</v>
+        <v>29</v>
       </c>
       <c r="S80" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="T80" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="U80" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="V80" t="s">
-        <v>29</v>
+        <v>479</v>
       </c>
       <c r="W80" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="B81" t="s">
         <v>23</v>
       </c>
       <c r="C81" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="D81">
         <v>91207</v>
@@ -8254,19 +8269,19 @@
         <v>418</v>
       </c>
       <c r="F81" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="G81" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="H81" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="I81" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="J81" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K81" t="s">
         <v>47</v>
@@ -8281,57 +8296,57 @@
         <v>30</v>
       </c>
       <c r="O81" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="P81" t="s">
-        <v>29</v>
+        <v>485</v>
       </c>
       <c r="Q81" t="s">
-        <v>29</v>
+        <v>485</v>
       </c>
       <c r="R81" t="s">
-        <v>57</v>
+        <v>485</v>
       </c>
       <c r="S81" t="s">
-        <v>57</v>
+        <v>485</v>
       </c>
       <c r="T81" t="s">
-        <v>57</v>
+        <v>485</v>
       </c>
       <c r="U81" t="s">
-        <v>57</v>
+        <v>485</v>
       </c>
       <c r="V81" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="W81" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="B82" t="s">
         <v>23</v>
       </c>
       <c r="C82" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="D82">
-        <v>91227</v>
+        <v>91207</v>
       </c>
       <c r="E82" t="s">
-        <v>493</v>
+        <v>418</v>
       </c>
       <c r="F82" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="G82" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="H82" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="I82" t="s">
         <v>29</v>
@@ -8361,33 +8376,33 @@
         <v>29</v>
       </c>
       <c r="R82" t="s">
-        <v>175</v>
+        <v>57</v>
       </c>
       <c r="S82" t="s">
-        <v>175</v>
+        <v>57</v>
       </c>
       <c r="T82" t="s">
-        <v>175</v>
+        <v>57</v>
       </c>
       <c r="U82" t="s">
-        <v>497</v>
+        <v>57</v>
       </c>
       <c r="V82" t="s">
-        <v>497</v>
+        <v>57</v>
       </c>
       <c r="W82" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="B83" t="s">
         <v>23</v>
       </c>
       <c r="C83" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="D83">
         <v>91227</v>
@@ -8396,16 +8411,16 @@
         <v>493</v>
       </c>
       <c r="F83" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="G83" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="H83" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="I83" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J83" t="s">
         <v>29</v>
@@ -8426,39 +8441,39 @@
         <v>31</v>
       </c>
       <c r="P83" t="s">
-        <v>503</v>
+        <v>29</v>
       </c>
       <c r="Q83" t="s">
         <v>29</v>
       </c>
       <c r="R83" t="s">
-        <v>503</v>
+        <v>175</v>
       </c>
       <c r="S83" t="s">
-        <v>503</v>
+        <v>175</v>
       </c>
       <c r="T83" t="s">
-        <v>503</v>
+        <v>175</v>
       </c>
       <c r="U83" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="V83" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="W83" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="B84" t="s">
         <v>23</v>
       </c>
       <c r="C84" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D84">
         <v>91227</v>
@@ -8467,25 +8482,25 @@
         <v>493</v>
       </c>
       <c r="F84" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="G84" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="H84" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="I84" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="J84" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K84" t="s">
         <v>47</v>
       </c>
       <c r="L84" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="M84" t="s">
         <v>41</v>
@@ -8497,63 +8512,63 @@
         <v>31</v>
       </c>
       <c r="P84" t="s">
-        <v>29</v>
+        <v>503</v>
       </c>
       <c r="Q84" t="s">
-        <v>509</v>
+        <v>29</v>
       </c>
       <c r="R84" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="S84" t="s">
-        <v>29</v>
+        <v>503</v>
       </c>
       <c r="T84" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="U84" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="V84" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="W84" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="B85" t="s">
         <v>23</v>
       </c>
       <c r="C85" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="D85">
-        <v>91284</v>
+        <v>91227</v>
       </c>
       <c r="E85" t="s">
-        <v>513</v>
+        <v>493</v>
       </c>
       <c r="F85" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="G85" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="H85" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="I85" t="s">
         <v>29</v>
       </c>
       <c r="J85" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K85" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L85" t="s">
         <v>29</v>
@@ -8571,51 +8586,51 @@
         <v>29</v>
       </c>
       <c r="Q85" t="s">
-        <v>29</v>
+        <v>509</v>
       </c>
       <c r="R85" t="s">
-        <v>29</v>
+        <v>509</v>
       </c>
       <c r="S85" t="s">
         <v>29</v>
       </c>
       <c r="T85" t="s">
-        <v>56</v>
+        <v>509</v>
       </c>
       <c r="U85" t="s">
-        <v>163</v>
+        <v>509</v>
       </c>
       <c r="V85" t="s">
-        <v>163</v>
+        <v>510</v>
       </c>
       <c r="W85" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="B86" t="s">
         <v>23</v>
       </c>
       <c r="C86" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="D86">
-        <v>91233</v>
+        <v>91284</v>
       </c>
       <c r="E86" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="F86" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="G86" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="H86" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="I86" t="s">
         <v>29</v>
@@ -8633,7 +8648,7 @@
         <v>41</v>
       </c>
       <c r="N86" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O86" t="s">
         <v>31</v>
@@ -8651,60 +8666,60 @@
         <v>29</v>
       </c>
       <c r="T86" t="s">
-        <v>523</v>
+        <v>56</v>
       </c>
       <c r="U86" t="s">
-        <v>29</v>
+        <v>163</v>
       </c>
       <c r="V86" t="s">
-        <v>524</v>
+        <v>163</v>
       </c>
       <c r="W86" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="B87" t="s">
-        <v>249</v>
+        <v>23</v>
       </c>
       <c r="C87" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="D87">
-        <v>91242</v>
+        <v>91233</v>
       </c>
       <c r="E87" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="F87" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="G87" t="s">
-        <v>27</v>
+        <v>521</v>
       </c>
       <c r="H87" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="I87" t="s">
         <v>29</v>
       </c>
       <c r="J87" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K87" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L87" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="M87" t="s">
         <v>41</v>
       </c>
       <c r="N87" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O87" t="s">
         <v>31</v>
@@ -8713,36 +8728,36 @@
         <v>29</v>
       </c>
       <c r="Q87" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="R87" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="S87" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="T87" t="s">
-        <v>71</v>
+        <v>523</v>
       </c>
       <c r="U87" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="V87" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="W87" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="B88" t="s">
-        <v>23</v>
+        <v>249</v>
       </c>
       <c r="C88" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="D88">
         <v>91242</v>
@@ -8751,19 +8766,19 @@
         <v>527</v>
       </c>
       <c r="F88" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="G88" t="s">
         <v>27</v>
       </c>
       <c r="H88" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="I88" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J88" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K88" t="s">
         <v>47</v>
@@ -8781,63 +8796,63 @@
         <v>31</v>
       </c>
       <c r="P88" t="s">
-        <v>535</v>
+        <v>29</v>
       </c>
       <c r="Q88" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="R88" t="s">
-        <v>535</v>
+        <v>71</v>
       </c>
       <c r="S88" t="s">
-        <v>535</v>
+        <v>71</v>
       </c>
       <c r="T88" t="s">
-        <v>234</v>
+        <v>71</v>
       </c>
       <c r="U88" t="s">
-        <v>234</v>
+        <v>71</v>
       </c>
       <c r="V88" t="s">
-        <v>234</v>
+        <v>530</v>
       </c>
       <c r="W88" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="B89" t="s">
         <v>23</v>
       </c>
       <c r="C89" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D89">
-        <v>91287</v>
+        <v>91242</v>
       </c>
       <c r="E89" t="s">
-        <v>538</v>
+        <v>527</v>
       </c>
       <c r="F89" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="G89" t="s">
-        <v>540</v>
+        <v>27</v>
       </c>
       <c r="H89" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="I89" t="s">
         <v>38</v>
       </c>
       <c r="J89" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K89" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L89" t="s">
         <v>40</v>
@@ -8852,39 +8867,39 @@
         <v>31</v>
       </c>
       <c r="P89" t="s">
-        <v>292</v>
+        <v>535</v>
       </c>
       <c r="Q89" t="s">
-        <v>292</v>
+        <v>29</v>
       </c>
       <c r="R89" t="s">
-        <v>29</v>
+        <v>535</v>
       </c>
       <c r="S89" t="s">
-        <v>292</v>
+        <v>535</v>
       </c>
       <c r="T89" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
       <c r="U89" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
       <c r="V89" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
       <c r="W89" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="B90" t="s">
         <v>23</v>
       </c>
       <c r="C90" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="D90">
         <v>91287</v>
@@ -8893,28 +8908,28 @@
         <v>538</v>
       </c>
       <c r="F90" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="G90" t="s">
-        <v>27</v>
+        <v>540</v>
       </c>
       <c r="H90" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="I90" t="s">
         <v>38</v>
       </c>
       <c r="J90" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K90" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L90" t="s">
         <v>40</v>
       </c>
       <c r="M90" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="N90" t="s">
         <v>30</v>
@@ -8923,39 +8938,39 @@
         <v>31</v>
       </c>
       <c r="P90" t="s">
-        <v>546</v>
+        <v>292</v>
       </c>
       <c r="Q90" t="s">
-        <v>29</v>
+        <v>292</v>
       </c>
       <c r="R90" t="s">
-        <v>546</v>
+        <v>29</v>
       </c>
       <c r="S90" t="s">
-        <v>546</v>
+        <v>292</v>
       </c>
       <c r="T90" t="s">
-        <v>29</v>
+        <v>292</v>
       </c>
       <c r="U90" t="s">
-        <v>546</v>
+        <v>292</v>
       </c>
       <c r="V90" t="s">
-        <v>547</v>
+        <v>292</v>
       </c>
       <c r="W90" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="B91" t="s">
         <v>23</v>
       </c>
       <c r="C91" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="D91">
         <v>91287</v>
@@ -8964,19 +8979,19 @@
         <v>538</v>
       </c>
       <c r="F91" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="G91" t="s">
-        <v>551</v>
+        <v>27</v>
       </c>
       <c r="H91" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="I91" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="J91" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K91" t="s">
         <v>47</v>
@@ -8985,7 +9000,7 @@
         <v>40</v>
       </c>
       <c r="M91" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="N91" t="s">
         <v>30</v>
@@ -8994,63 +9009,63 @@
         <v>31</v>
       </c>
       <c r="P91" t="s">
-        <v>29</v>
+        <v>546</v>
       </c>
       <c r="Q91" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="R91" t="s">
-        <v>71</v>
+        <v>546</v>
       </c>
       <c r="S91" t="s">
-        <v>71</v>
+        <v>546</v>
       </c>
       <c r="T91" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="U91" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="V91" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="W91" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="B92" t="s">
         <v>23</v>
       </c>
       <c r="C92" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="D92">
-        <v>91224</v>
+        <v>91287</v>
       </c>
       <c r="E92" t="s">
-        <v>556</v>
+        <v>538</v>
       </c>
       <c r="F92" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="G92" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="H92" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="I92" t="s">
         <v>29</v>
       </c>
       <c r="J92" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K92" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L92" t="s">
         <v>40</v>
@@ -9068,36 +9083,36 @@
         <v>29</v>
       </c>
       <c r="Q92" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="R92" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="S92" t="s">
-        <v>560</v>
+        <v>71</v>
       </c>
       <c r="T92" t="s">
-        <v>560</v>
+        <v>71</v>
       </c>
       <c r="U92" t="s">
-        <v>42</v>
+        <v>553</v>
       </c>
       <c r="V92" t="s">
-        <v>42</v>
+        <v>553</v>
       </c>
       <c r="W92" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="B93" t="s">
         <v>23</v>
       </c>
       <c r="C93" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
       <c r="D93">
         <v>91224</v>
@@ -9106,25 +9121,25 @@
         <v>556</v>
       </c>
       <c r="F93" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="G93" t="s">
-        <v>27</v>
+        <v>558</v>
       </c>
       <c r="H93" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="I93" t="s">
         <v>29</v>
       </c>
       <c r="J93" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K93" t="s">
         <v>29</v>
       </c>
       <c r="L93" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="M93" t="s">
         <v>41</v>
@@ -9139,36 +9154,36 @@
         <v>29</v>
       </c>
       <c r="Q93" t="s">
-        <v>225</v>
+        <v>29</v>
       </c>
       <c r="R93" t="s">
         <v>29</v>
       </c>
       <c r="S93" t="s">
-        <v>29</v>
+        <v>560</v>
       </c>
       <c r="T93" t="s">
-        <v>225</v>
+        <v>560</v>
       </c>
       <c r="U93" t="s">
-        <v>401</v>
+        <v>42</v>
       </c>
       <c r="V93" t="s">
-        <v>565</v>
+        <v>42</v>
       </c>
       <c r="W93" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="B94" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="C94" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="D94">
         <v>91224</v>
@@ -9177,13 +9192,13 @@
         <v>556</v>
       </c>
       <c r="F94" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="G94" t="s">
         <v>27</v>
       </c>
       <c r="H94" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="I94" t="s">
         <v>29</v>
@@ -9192,10 +9207,10 @@
         <v>39</v>
       </c>
       <c r="K94" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L94" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="M94" t="s">
         <v>41</v>
@@ -9210,57 +9225,57 @@
         <v>29</v>
       </c>
       <c r="Q94" t="s">
-        <v>106</v>
+        <v>225</v>
       </c>
       <c r="R94" t="s">
-        <v>106</v>
+        <v>29</v>
       </c>
       <c r="S94" t="s">
-        <v>106</v>
+        <v>29</v>
       </c>
       <c r="T94" t="s">
-        <v>106</v>
+        <v>225</v>
       </c>
       <c r="U94" t="s">
-        <v>106</v>
+        <v>401</v>
       </c>
       <c r="V94" t="s">
-        <v>106</v>
+        <v>565</v>
       </c>
       <c r="W94" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="B95" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="C95" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="D95">
-        <v>90552</v>
+        <v>91224</v>
       </c>
       <c r="E95" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="F95" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="G95" t="s">
-        <v>574</v>
+        <v>27</v>
       </c>
       <c r="H95" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="I95" t="s">
         <v>29</v>
       </c>
       <c r="J95" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K95" t="s">
         <v>47</v>
@@ -9281,36 +9296,36 @@
         <v>29</v>
       </c>
       <c r="Q95" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="R95" t="s">
-        <v>286</v>
+        <v>106</v>
       </c>
       <c r="S95" t="s">
-        <v>286</v>
+        <v>106</v>
       </c>
       <c r="T95" t="s">
-        <v>286</v>
+        <v>106</v>
       </c>
       <c r="U95" t="s">
-        <v>286</v>
+        <v>106</v>
       </c>
       <c r="V95" t="s">
-        <v>286</v>
+        <v>106</v>
       </c>
       <c r="W95" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="B96" t="s">
         <v>23</v>
       </c>
       <c r="C96" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="D96">
         <v>90552</v>
@@ -9319,13 +9334,13 @@
         <v>572</v>
       </c>
       <c r="F96" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="G96" t="s">
-        <v>27</v>
+        <v>574</v>
       </c>
       <c r="H96" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="I96" t="s">
         <v>29</v>
@@ -9355,33 +9370,33 @@
         <v>29</v>
       </c>
       <c r="R96" t="s">
-        <v>42</v>
+        <v>286</v>
       </c>
       <c r="S96" t="s">
-        <v>42</v>
+        <v>286</v>
       </c>
       <c r="T96" t="s">
-        <v>42</v>
+        <v>286</v>
       </c>
       <c r="U96" t="s">
-        <v>42</v>
+        <v>286</v>
       </c>
       <c r="V96" t="s">
-        <v>42</v>
+        <v>286</v>
       </c>
       <c r="W96" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="B97" t="s">
         <v>23</v>
       </c>
       <c r="C97" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="D97">
         <v>90552</v>
@@ -9390,22 +9405,22 @@
         <v>572</v>
       </c>
       <c r="F97" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="G97" t="s">
-        <v>583</v>
+        <v>27</v>
       </c>
       <c r="H97" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="I97" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J97" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K97" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L97" t="s">
         <v>40</v>
@@ -9420,63 +9435,63 @@
         <v>31</v>
       </c>
       <c r="P97" t="s">
-        <v>585</v>
+        <v>29</v>
       </c>
       <c r="Q97" t="s">
-        <v>585</v>
+        <v>29</v>
       </c>
       <c r="R97" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="S97" t="s">
-        <v>585</v>
+        <v>42</v>
       </c>
       <c r="T97" t="s">
-        <v>585</v>
+        <v>42</v>
       </c>
       <c r="U97" t="s">
-        <v>585</v>
+        <v>42</v>
       </c>
       <c r="V97" t="s">
-        <v>586</v>
+        <v>42</v>
       </c>
       <c r="W97" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
       <c r="B98" t="s">
         <v>23</v>
       </c>
       <c r="C98" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
       <c r="D98">
-        <v>91245</v>
+        <v>90552</v>
       </c>
       <c r="E98" t="s">
-        <v>589</v>
+        <v>572</v>
       </c>
       <c r="F98" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="G98" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
       <c r="H98" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="I98" t="s">
         <v>38</v>
       </c>
       <c r="J98" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K98" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L98" t="s">
         <v>40</v>
@@ -9491,39 +9506,39 @@
         <v>31</v>
       </c>
       <c r="P98" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="Q98" t="s">
-        <v>29</v>
+        <v>585</v>
       </c>
       <c r="R98" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="S98" t="s">
-        <v>42</v>
+        <v>585</v>
       </c>
       <c r="T98" t="s">
-        <v>42</v>
+        <v>585</v>
       </c>
       <c r="U98" t="s">
-        <v>594</v>
+        <v>585</v>
       </c>
       <c r="V98" t="s">
-        <v>595</v>
+        <v>586</v>
       </c>
       <c r="W98" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>596</v>
+        <v>587</v>
       </c>
       <c r="B99" t="s">
         <v>23</v>
       </c>
       <c r="C99" t="s">
-        <v>597</v>
+        <v>588</v>
       </c>
       <c r="D99">
         <v>91245</v>
@@ -9532,16 +9547,16 @@
         <v>589</v>
       </c>
       <c r="F99" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="G99" t="s">
-        <v>27</v>
+        <v>591</v>
       </c>
       <c r="H99" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
       <c r="I99" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="J99" t="s">
         <v>29</v>
@@ -9562,39 +9577,39 @@
         <v>31</v>
       </c>
       <c r="P99" t="s">
-        <v>29</v>
+        <v>593</v>
       </c>
       <c r="Q99" t="s">
         <v>29</v>
       </c>
       <c r="R99" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="S99" t="s">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="T99" t="s">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="U99" t="s">
-        <v>104</v>
+        <v>594</v>
       </c>
       <c r="V99" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="W99" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>647</v>
+        <v>596</v>
       </c>
       <c r="B100" t="s">
         <v>23</v>
       </c>
       <c r="C100" t="s">
-        <v>648</v>
+        <v>597</v>
       </c>
       <c r="D100">
         <v>91245</v>
@@ -9602,14 +9617,14 @@
       <c r="E100" t="s">
         <v>589</v>
       </c>
-      <c r="F100" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="G100" s="4" t="s">
-        <v>651</v>
-      </c>
-      <c r="H100" s="4" t="s">
-        <v>650</v>
+      <c r="F100" t="s">
+        <v>598</v>
+      </c>
+      <c r="G100" t="s">
+        <v>27</v>
+      </c>
+      <c r="H100" t="s">
+        <v>599</v>
       </c>
       <c r="I100" t="s">
         <v>29</v>
@@ -9639,48 +9654,48 @@
         <v>29</v>
       </c>
       <c r="R100" t="s">
-        <v>652</v>
+        <v>71</v>
       </c>
       <c r="S100" t="s">
-        <v>586</v>
+        <v>104</v>
       </c>
       <c r="T100" t="s">
-        <v>586</v>
+        <v>104</v>
       </c>
       <c r="U100" t="s">
-        <v>586</v>
+        <v>104</v>
       </c>
       <c r="V100" t="s">
-        <v>586</v>
+        <v>600</v>
       </c>
       <c r="W100" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>601</v>
+        <v>647</v>
       </c>
       <c r="B101" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="C101" t="s">
-        <v>602</v>
+        <v>648</v>
       </c>
       <c r="D101">
-        <v>91247</v>
+        <v>91245</v>
       </c>
       <c r="E101" t="s">
-        <v>603</v>
-      </c>
-      <c r="F101" t="s">
-        <v>604</v>
-      </c>
-      <c r="G101" t="s">
-        <v>27</v>
-      </c>
-      <c r="H101" t="s">
-        <v>605</v>
+        <v>589</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="G101" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="H101" s="4" t="s">
+        <v>650</v>
       </c>
       <c r="I101" t="s">
         <v>29</v>
@@ -9689,13 +9704,13 @@
         <v>29</v>
       </c>
       <c r="K101" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L101" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="M101" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="N101" t="s">
         <v>30</v>
@@ -9710,33 +9725,33 @@
         <v>29</v>
       </c>
       <c r="R101" t="s">
-        <v>29</v>
+        <v>652</v>
       </c>
       <c r="S101" t="s">
-        <v>29</v>
+        <v>586</v>
       </c>
       <c r="T101" t="s">
-        <v>29</v>
+        <v>586</v>
       </c>
       <c r="U101" t="s">
-        <v>72</v>
+        <v>586</v>
       </c>
       <c r="V101" t="s">
-        <v>606</v>
+        <v>586</v>
       </c>
       <c r="W101" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="B102" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C102" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="D102">
         <v>91247</v>
@@ -9745,28 +9760,28 @@
         <v>603</v>
       </c>
       <c r="F102" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="G102" t="s">
-        <v>610</v>
+        <v>27</v>
       </c>
       <c r="H102" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="I102" t="s">
         <v>29</v>
       </c>
       <c r="J102" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K102" t="s">
         <v>29</v>
       </c>
       <c r="L102" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="M102" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="N102" t="s">
         <v>30</v>
@@ -9778,36 +9793,36 @@
         <v>29</v>
       </c>
       <c r="Q102" t="s">
-        <v>612</v>
+        <v>29</v>
       </c>
       <c r="R102" t="s">
         <v>29</v>
       </c>
       <c r="S102" t="s">
-        <v>612</v>
+        <v>29</v>
       </c>
       <c r="T102" t="s">
-        <v>612</v>
+        <v>29</v>
       </c>
       <c r="U102" t="s">
-        <v>612</v>
+        <v>72</v>
       </c>
       <c r="V102" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="W102" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="B103" t="s">
         <v>23</v>
       </c>
       <c r="C103" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="D103">
         <v>91247</v>
@@ -9816,25 +9831,25 @@
         <v>603</v>
       </c>
       <c r="F103" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="G103" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="H103" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="I103" t="s">
         <v>29</v>
       </c>
       <c r="J103" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K103" t="s">
         <v>29</v>
       </c>
       <c r="L103" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="M103" t="s">
         <v>41</v>
@@ -9849,51 +9864,51 @@
         <v>29</v>
       </c>
       <c r="Q103" t="s">
-        <v>29</v>
+        <v>612</v>
       </c>
       <c r="R103" t="s">
         <v>29</v>
       </c>
       <c r="S103" t="s">
-        <v>29</v>
+        <v>612</v>
       </c>
       <c r="T103" t="s">
-        <v>469</v>
+        <v>612</v>
       </c>
       <c r="U103" t="s">
-        <v>469</v>
+        <v>612</v>
       </c>
       <c r="V103" t="s">
-        <v>57</v>
+        <v>612</v>
       </c>
       <c r="W103" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="B104" t="s">
         <v>23</v>
       </c>
       <c r="C104" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="D104">
-        <v>91367</v>
+        <v>91247</v>
       </c>
       <c r="E104" t="s">
-        <v>620</v>
+        <v>603</v>
       </c>
       <c r="F104" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="G104" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="H104" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="I104" t="s">
         <v>29</v>
@@ -9905,7 +9920,7 @@
         <v>29</v>
       </c>
       <c r="L104" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="M104" t="s">
         <v>41</v>
@@ -9926,30 +9941,30 @@
         <v>29</v>
       </c>
       <c r="S104" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="T104" t="s">
-        <v>72</v>
+        <v>469</v>
       </c>
       <c r="U104" t="s">
-        <v>72</v>
+        <v>469</v>
       </c>
       <c r="V104" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="W104" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="B105" t="s">
         <v>23</v>
       </c>
       <c r="C105" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="D105">
         <v>91367</v>
@@ -9958,22 +9973,22 @@
         <v>620</v>
       </c>
       <c r="F105" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="G105" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="H105" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="I105" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J105" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K105" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L105" t="s">
         <v>40</v>
@@ -9985,30 +10000,101 @@
         <v>30</v>
       </c>
       <c r="O105" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P105" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>29</v>
+      </c>
+      <c r="R105" t="s">
+        <v>29</v>
+      </c>
+      <c r="S105" t="s">
+        <v>71</v>
+      </c>
+      <c r="T105" t="s">
+        <v>72</v>
+      </c>
+      <c r="U105" t="s">
+        <v>72</v>
+      </c>
+      <c r="V105" t="s">
+        <v>72</v>
+      </c>
+      <c r="W105" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>624</v>
+      </c>
+      <c r="B106" t="s">
+        <v>23</v>
+      </c>
+      <c r="C106" t="s">
+        <v>625</v>
+      </c>
+      <c r="D106">
+        <v>91367</v>
+      </c>
+      <c r="E106" t="s">
+        <v>620</v>
+      </c>
+      <c r="F106" t="s">
+        <v>626</v>
+      </c>
+      <c r="G106" t="s">
+        <v>627</v>
+      </c>
+      <c r="H106" t="s">
+        <v>628</v>
+      </c>
+      <c r="I106" t="s">
+        <v>38</v>
+      </c>
+      <c r="J106" t="s">
+        <v>39</v>
+      </c>
+      <c r="K106" t="s">
+        <v>47</v>
+      </c>
+      <c r="L106" t="s">
+        <v>40</v>
+      </c>
+      <c r="M106" t="s">
+        <v>41</v>
+      </c>
+      <c r="N106" t="s">
+        <v>30</v>
+      </c>
+      <c r="O106" t="s">
+        <v>29</v>
+      </c>
+      <c r="P106" t="s">
         <v>629</v>
       </c>
-      <c r="Q105" t="s">
+      <c r="Q106" t="s">
         <v>629</v>
       </c>
-      <c r="R105" t="s">
+      <c r="R106" t="s">
         <v>629</v>
       </c>
-      <c r="S105" t="s">
+      <c r="S106" t="s">
         <v>629</v>
       </c>
-      <c r="T105" t="s">
+      <c r="T106" t="s">
         <v>629</v>
       </c>
-      <c r="U105" t="s">
+      <c r="U106" t="s">
         <v>630</v>
       </c>
-      <c r="V105" t="s">
-        <v>29</v>
-      </c>
-      <c r="W105" t="s">
+      <c r="V106" t="s">
+        <v>29</v>
+      </c>
+      <c r="W106" t="s">
         <v>27</v>
       </c>
     </row>
@@ -10016,15 +10102,16 @@
   <hyperlinks>
     <hyperlink ref="H58" r:id="rId1" xr:uid="{3518E2E3-45F1-448A-93F8-FA096D84A577}"/>
     <hyperlink ref="G58" r:id="rId2" xr:uid="{7220F707-B88F-4FDE-AEBA-ED4F716E05CE}"/>
-    <hyperlink ref="H79" r:id="rId3" xr:uid="{AD9CFEB0-515E-47DE-A619-8A0566327566}"/>
-    <hyperlink ref="G67" r:id="rId4" xr:uid="{C5402745-E279-4144-A7EA-01FCE7A4E404}"/>
-    <hyperlink ref="H67" r:id="rId5" xr:uid="{679F818E-03B4-4BF2-B47A-7E4540C537AF}"/>
-    <hyperlink ref="H100" r:id="rId6" xr:uid="{64B05FEF-865E-4E04-B288-9B0F0E91EB19}"/>
-    <hyperlink ref="G100" r:id="rId7" xr:uid="{1C619C93-40F6-455D-B3C4-D8F5DA0E79E2}"/>
+    <hyperlink ref="H80" r:id="rId3" xr:uid="{AD9CFEB0-515E-47DE-A619-8A0566327566}"/>
+    <hyperlink ref="G68" r:id="rId4" xr:uid="{C5402745-E279-4144-A7EA-01FCE7A4E404}"/>
+    <hyperlink ref="H68" r:id="rId5" xr:uid="{679F818E-03B4-4BF2-B47A-7E4540C537AF}"/>
+    <hyperlink ref="H101" r:id="rId6" xr:uid="{64B05FEF-865E-4E04-B288-9B0F0E91EB19}"/>
+    <hyperlink ref="G101" r:id="rId7" xr:uid="{1C619C93-40F6-455D-B3C4-D8F5DA0E79E2}"/>
+    <hyperlink ref="H66" r:id="rId8" xr:uid="{811F14D2-8625-407A-A363-4868792D85E3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
@@ -10035,7 +10122,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Schlosskeller in Lauf added
</commit_message>
<xml_diff>
--- a/cfg/pubfinder_list_NLA.xlsx
+++ b/cfg/pubfinder_list_NLA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_dev\pubfinder_V2\cfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2F7397-9C24-4531-A9A8-8DA728C0DB52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9578AE34-1123-43CC-9D2B-5A4FF8251A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{75E81789-C525-4005-96BA-B080353C5F6C}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">pubfinder_list_NLA!$A$1:$W$107</definedName>
+    <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">pubfinder_list_NLA!$A$1:$W$108</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2366" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2376" uniqueCount="672">
   <si>
     <t>Name</t>
   </si>
@@ -2043,6 +2043,27 @@
   </si>
   <si>
     <t>09:00 - 00:00</t>
+  </si>
+  <si>
+    <t>Schlosskeller</t>
+  </si>
+  <si>
+    <t>Cocktail</t>
+  </si>
+  <si>
+    <t>Bergstr. 2</t>
+  </si>
+  <si>
+    <t>+499123966635</t>
+  </si>
+  <si>
+    <t>www.schlosskeller-lauf.de</t>
+  </si>
+  <si>
+    <t>18:00 - 01:00</t>
+  </si>
+  <si>
+    <t>18:00 - 03:00</t>
   </si>
 </sst>
 </file>
@@ -2222,8 +2243,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C4BF8B3-CB62-48F7-AAC2-6E12CB367C86}" name="pubfinder_list_NLA_ok" displayName="pubfinder_list_NLA_ok" ref="A1:W107" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:W107" xr:uid="{1C4BF8B3-CB62-48F7-AAC2-6E12CB367C86}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C4BF8B3-CB62-48F7-AAC2-6E12CB367C86}" name="pubfinder_list_NLA_ok" displayName="pubfinder_list_NLA_ok" ref="A1:W108" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:W108" xr:uid="{1C4BF8B3-CB62-48F7-AAC2-6E12CB367C86}"/>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{92103B2C-FCC3-42D2-95DB-A3F77D77EC29}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="21"/>
     <tableColumn id="2" xr3:uid="{86208C35-2046-4F53-B583-F5FD55ED84C8}" uniqueName="2" name="Typ" queryTableFieldId="2" dataDxfId="20"/>
@@ -2570,10 +2591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F2D7F2-8E23-4C59-B8E8-2949683E6C83}">
-  <dimension ref="A1:W107"/>
+  <dimension ref="A1:W108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J49" workbookViewId="0">
-      <selection activeCell="X69" sqref="X69"/>
+    <sheetView tabSelected="1" topLeftCell="I64" workbookViewId="0">
+      <selection activeCell="T79" sqref="T79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8136,13 +8157,13 @@
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>470</v>
+        <v>665</v>
       </c>
       <c r="B79" t="s">
-        <v>66</v>
+        <v>666</v>
       </c>
       <c r="C79" t="s">
-        <v>471</v>
+        <v>667</v>
       </c>
       <c r="D79">
         <v>91207</v>
@@ -8150,23 +8171,23 @@
       <c r="E79" t="s">
         <v>418</v>
       </c>
-      <c r="F79" t="s">
-        <v>445</v>
+      <c r="F79" s="2" t="s">
+        <v>668</v>
       </c>
       <c r="G79" t="s">
         <v>27</v>
       </c>
-      <c r="H79" t="s">
-        <v>472</v>
+      <c r="H79" s="4" t="s">
+        <v>669</v>
       </c>
       <c r="I79" t="s">
         <v>29</v>
       </c>
       <c r="J79" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K79" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L79" t="s">
         <v>40</v>
@@ -8178,28 +8199,28 @@
         <v>30</v>
       </c>
       <c r="O79" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P79" t="s">
         <v>29</v>
       </c>
       <c r="Q79" t="s">
-        <v>232</v>
+        <v>29</v>
       </c>
       <c r="R79" t="s">
-        <v>232</v>
+        <v>29</v>
       </c>
       <c r="S79" t="s">
-        <v>232</v>
+        <v>670</v>
       </c>
       <c r="T79" t="s">
-        <v>232</v>
+        <v>671</v>
       </c>
       <c r="U79" t="s">
-        <v>253</v>
+        <v>671</v>
       </c>
       <c r="V79" t="s">
-        <v>29</v>
+        <v>670</v>
       </c>
       <c r="W79" t="s">
         <v>27</v>
@@ -8207,13 +8228,13 @@
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B80" t="s">
         <v>66</v>
       </c>
       <c r="C80" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D80">
         <v>91207</v>
@@ -8228,7 +8249,7 @@
         <v>27</v>
       </c>
       <c r="H80" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="I80" t="s">
         <v>29</v>
@@ -8249,28 +8270,28 @@
         <v>30</v>
       </c>
       <c r="O80" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="P80" t="s">
         <v>29</v>
       </c>
       <c r="Q80" t="s">
-        <v>292</v>
+        <v>232</v>
       </c>
       <c r="R80" t="s">
-        <v>292</v>
+        <v>232</v>
       </c>
       <c r="S80" t="s">
-        <v>292</v>
+        <v>232</v>
       </c>
       <c r="T80" t="s">
-        <v>292</v>
+        <v>232</v>
       </c>
       <c r="U80" t="s">
-        <v>292</v>
+        <v>253</v>
       </c>
       <c r="V80" t="s">
-        <v>292</v>
+        <v>29</v>
       </c>
       <c r="W80" t="s">
         <v>27</v>
@@ -8278,13 +8299,13 @@
     </row>
     <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B81" t="s">
         <v>66</v>
       </c>
       <c r="C81" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="D81">
         <v>91207</v>
@@ -8293,22 +8314,22 @@
         <v>418</v>
       </c>
       <c r="F81" t="s">
-        <v>478</v>
+        <v>445</v>
       </c>
       <c r="G81" t="s">
         <v>27</v>
       </c>
-      <c r="H81" s="4" t="s">
-        <v>639</v>
+      <c r="H81" t="s">
+        <v>475</v>
       </c>
       <c r="I81" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J81" t="s">
         <v>39</v>
       </c>
       <c r="K81" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L81" t="s">
         <v>40</v>
@@ -8323,25 +8344,25 @@
         <v>31</v>
       </c>
       <c r="P81" t="s">
-        <v>479</v>
+        <v>29</v>
       </c>
       <c r="Q81" t="s">
-        <v>479</v>
+        <v>292</v>
       </c>
       <c r="R81" t="s">
-        <v>29</v>
+        <v>292</v>
       </c>
       <c r="S81" t="s">
-        <v>479</v>
+        <v>292</v>
       </c>
       <c r="T81" t="s">
-        <v>479</v>
+        <v>292</v>
       </c>
       <c r="U81" t="s">
-        <v>479</v>
+        <v>292</v>
       </c>
       <c r="V81" t="s">
-        <v>479</v>
+        <v>292</v>
       </c>
       <c r="W81" t="s">
         <v>27</v>
@@ -8349,13 +8370,13 @@
     </row>
     <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B82" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="C82" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="D82">
         <v>91207</v>
@@ -8364,13 +8385,13 @@
         <v>418</v>
       </c>
       <c r="F82" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="G82" t="s">
-        <v>483</v>
-      </c>
-      <c r="H82" t="s">
-        <v>484</v>
+        <v>27</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>639</v>
       </c>
       <c r="I82" t="s">
         <v>38</v>
@@ -8379,7 +8400,7 @@
         <v>39</v>
       </c>
       <c r="K82" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L82" t="s">
         <v>40</v>
@@ -8391,28 +8412,28 @@
         <v>30</v>
       </c>
       <c r="O82" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P82" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="Q82" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="R82" t="s">
-        <v>485</v>
+        <v>29</v>
       </c>
       <c r="S82" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="T82" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="U82" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="V82" t="s">
-        <v>29</v>
+        <v>479</v>
       </c>
       <c r="W82" t="s">
         <v>27</v>
@@ -8420,13 +8441,13 @@
     </row>
     <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="B83" t="s">
         <v>23</v>
       </c>
       <c r="C83" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="D83">
         <v>91207</v>
@@ -8435,19 +8456,19 @@
         <v>418</v>
       </c>
       <c r="F83" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="G83" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="H83" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="I83" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="J83" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K83" t="s">
         <v>47</v>
@@ -8462,28 +8483,28 @@
         <v>30</v>
       </c>
       <c r="O83" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="P83" t="s">
-        <v>29</v>
+        <v>485</v>
       </c>
       <c r="Q83" t="s">
-        <v>29</v>
+        <v>485</v>
       </c>
       <c r="R83" t="s">
-        <v>57</v>
+        <v>485</v>
       </c>
       <c r="S83" t="s">
-        <v>57</v>
+        <v>485</v>
       </c>
       <c r="T83" t="s">
-        <v>57</v>
+        <v>485</v>
       </c>
       <c r="U83" t="s">
-        <v>57</v>
+        <v>485</v>
       </c>
       <c r="V83" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="W83" t="s">
         <v>27</v>
@@ -8491,28 +8512,28 @@
     </row>
     <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="B84" t="s">
         <v>23</v>
       </c>
       <c r="C84" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="D84">
-        <v>91227</v>
+        <v>91207</v>
       </c>
       <c r="E84" t="s">
-        <v>493</v>
+        <v>418</v>
       </c>
       <c r="F84" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="G84" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="H84" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="I84" t="s">
         <v>29</v>
@@ -8542,19 +8563,19 @@
         <v>29</v>
       </c>
       <c r="R84" t="s">
-        <v>175</v>
+        <v>57</v>
       </c>
       <c r="S84" t="s">
-        <v>175</v>
+        <v>57</v>
       </c>
       <c r="T84" t="s">
-        <v>175</v>
+        <v>57</v>
       </c>
       <c r="U84" t="s">
-        <v>497</v>
+        <v>57</v>
       </c>
       <c r="V84" t="s">
-        <v>497</v>
+        <v>57</v>
       </c>
       <c r="W84" t="s">
         <v>27</v>
@@ -8562,13 +8583,13 @@
     </row>
     <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="B85" t="s">
         <v>23</v>
       </c>
       <c r="C85" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="D85">
         <v>91227</v>
@@ -8577,16 +8598,16 @@
         <v>493</v>
       </c>
       <c r="F85" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="G85" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="H85" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="I85" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J85" t="s">
         <v>29</v>
@@ -8607,25 +8628,25 @@
         <v>31</v>
       </c>
       <c r="P85" t="s">
-        <v>503</v>
+        <v>29</v>
       </c>
       <c r="Q85" t="s">
         <v>29</v>
       </c>
       <c r="R85" t="s">
-        <v>503</v>
+        <v>175</v>
       </c>
       <c r="S85" t="s">
-        <v>503</v>
+        <v>175</v>
       </c>
       <c r="T85" t="s">
-        <v>503</v>
+        <v>175</v>
       </c>
       <c r="U85" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="V85" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="W85" t="s">
         <v>27</v>
@@ -8633,13 +8654,13 @@
     </row>
     <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="B86" t="s">
         <v>23</v>
       </c>
       <c r="C86" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="D86">
         <v>91227</v>
@@ -8648,25 +8669,25 @@
         <v>493</v>
       </c>
       <c r="F86" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="G86" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="H86" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="I86" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="J86" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K86" t="s">
         <v>47</v>
       </c>
       <c r="L86" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="M86" t="s">
         <v>41</v>
@@ -8678,25 +8699,25 @@
         <v>31</v>
       </c>
       <c r="P86" t="s">
-        <v>29</v>
+        <v>503</v>
       </c>
       <c r="Q86" t="s">
-        <v>509</v>
+        <v>29</v>
       </c>
       <c r="R86" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="S86" t="s">
-        <v>29</v>
+        <v>503</v>
       </c>
       <c r="T86" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="U86" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="V86" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="W86" t="s">
         <v>27</v>
@@ -8704,37 +8725,37 @@
     </row>
     <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="B87" t="s">
         <v>23</v>
       </c>
       <c r="C87" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="D87">
-        <v>91284</v>
+        <v>91227</v>
       </c>
       <c r="E87" t="s">
-        <v>513</v>
+        <v>493</v>
       </c>
       <c r="F87" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="G87" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="H87" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="I87" t="s">
         <v>29</v>
       </c>
       <c r="J87" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K87" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L87" t="s">
         <v>29</v>
@@ -8752,22 +8773,22 @@
         <v>29</v>
       </c>
       <c r="Q87" t="s">
-        <v>29</v>
+        <v>509</v>
       </c>
       <c r="R87" t="s">
-        <v>29</v>
+        <v>509</v>
       </c>
       <c r="S87" t="s">
         <v>29</v>
       </c>
       <c r="T87" t="s">
-        <v>56</v>
+        <v>509</v>
       </c>
       <c r="U87" t="s">
-        <v>163</v>
+        <v>509</v>
       </c>
       <c r="V87" t="s">
-        <v>163</v>
+        <v>510</v>
       </c>
       <c r="W87" t="s">
         <v>27</v>
@@ -8775,28 +8796,28 @@
     </row>
     <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="B88" t="s">
         <v>23</v>
       </c>
       <c r="C88" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="D88">
-        <v>91233</v>
+        <v>91284</v>
       </c>
       <c r="E88" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="F88" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="G88" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="H88" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="I88" t="s">
         <v>29</v>
@@ -8814,7 +8835,7 @@
         <v>41</v>
       </c>
       <c r="N88" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O88" t="s">
         <v>31</v>
@@ -8832,13 +8853,13 @@
         <v>29</v>
       </c>
       <c r="T88" t="s">
-        <v>523</v>
+        <v>56</v>
       </c>
       <c r="U88" t="s">
-        <v>29</v>
+        <v>163</v>
       </c>
       <c r="V88" t="s">
-        <v>524</v>
+        <v>163</v>
       </c>
       <c r="W88" t="s">
         <v>27</v>
@@ -8846,46 +8867,46 @@
     </row>
     <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="B89" t="s">
-        <v>249</v>
+        <v>23</v>
       </c>
       <c r="C89" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="D89">
-        <v>91242</v>
+        <v>91233</v>
       </c>
       <c r="E89" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="F89" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="G89" t="s">
-        <v>27</v>
+        <v>521</v>
       </c>
       <c r="H89" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="I89" t="s">
         <v>29</v>
       </c>
       <c r="J89" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K89" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L89" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="M89" t="s">
         <v>41</v>
       </c>
       <c r="N89" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O89" t="s">
         <v>31</v>
@@ -8894,22 +8915,22 @@
         <v>29</v>
       </c>
       <c r="Q89" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="R89" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="S89" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="T89" t="s">
-        <v>71</v>
+        <v>523</v>
       </c>
       <c r="U89" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="V89" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="W89" t="s">
         <v>27</v>
@@ -8917,13 +8938,13 @@
     </row>
     <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="B90" t="s">
-        <v>23</v>
+        <v>249</v>
       </c>
       <c r="C90" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="D90">
         <v>91242</v>
@@ -8932,19 +8953,19 @@
         <v>527</v>
       </c>
       <c r="F90" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="G90" t="s">
         <v>27</v>
       </c>
       <c r="H90" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="I90" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J90" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K90" t="s">
         <v>47</v>
@@ -8962,25 +8983,25 @@
         <v>31</v>
       </c>
       <c r="P90" t="s">
-        <v>535</v>
+        <v>29</v>
       </c>
       <c r="Q90" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="R90" t="s">
-        <v>535</v>
+        <v>71</v>
       </c>
       <c r="S90" t="s">
-        <v>535</v>
+        <v>71</v>
       </c>
       <c r="T90" t="s">
-        <v>234</v>
+        <v>71</v>
       </c>
       <c r="U90" t="s">
-        <v>234</v>
+        <v>71</v>
       </c>
       <c r="V90" t="s">
-        <v>234</v>
+        <v>530</v>
       </c>
       <c r="W90" t="s">
         <v>27</v>
@@ -8988,37 +9009,37 @@
     </row>
     <row r="91" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="B91" t="s">
         <v>23</v>
       </c>
       <c r="C91" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D91">
-        <v>91287</v>
+        <v>91242</v>
       </c>
       <c r="E91" t="s">
-        <v>538</v>
+        <v>527</v>
       </c>
       <c r="F91" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="G91" t="s">
-        <v>540</v>
+        <v>27</v>
       </c>
       <c r="H91" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="I91" t="s">
         <v>38</v>
       </c>
       <c r="J91" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K91" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L91" t="s">
         <v>40</v>
@@ -9033,25 +9054,25 @@
         <v>31</v>
       </c>
       <c r="P91" t="s">
-        <v>292</v>
+        <v>535</v>
       </c>
       <c r="Q91" t="s">
-        <v>292</v>
+        <v>29</v>
       </c>
       <c r="R91" t="s">
-        <v>29</v>
+        <v>535</v>
       </c>
       <c r="S91" t="s">
-        <v>292</v>
+        <v>535</v>
       </c>
       <c r="T91" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
       <c r="U91" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
       <c r="V91" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
       <c r="W91" t="s">
         <v>27</v>
@@ -9059,13 +9080,13 @@
     </row>
     <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="B92" t="s">
         <v>23</v>
       </c>
       <c r="C92" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="D92">
         <v>91287</v>
@@ -9074,28 +9095,28 @@
         <v>538</v>
       </c>
       <c r="F92" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="G92" t="s">
-        <v>27</v>
+        <v>540</v>
       </c>
       <c r="H92" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="I92" t="s">
         <v>38</v>
       </c>
       <c r="J92" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K92" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L92" t="s">
         <v>40</v>
       </c>
       <c r="M92" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="N92" t="s">
         <v>30</v>
@@ -9104,25 +9125,25 @@
         <v>31</v>
       </c>
       <c r="P92" t="s">
-        <v>546</v>
+        <v>292</v>
       </c>
       <c r="Q92" t="s">
-        <v>29</v>
+        <v>292</v>
       </c>
       <c r="R92" t="s">
-        <v>546</v>
+        <v>29</v>
       </c>
       <c r="S92" t="s">
-        <v>546</v>
+        <v>292</v>
       </c>
       <c r="T92" t="s">
-        <v>29</v>
+        <v>292</v>
       </c>
       <c r="U92" t="s">
-        <v>546</v>
+        <v>292</v>
       </c>
       <c r="V92" t="s">
-        <v>547</v>
+        <v>292</v>
       </c>
       <c r="W92" t="s">
         <v>27</v>
@@ -9130,13 +9151,13 @@
     </row>
     <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="B93" t="s">
         <v>23</v>
       </c>
       <c r="C93" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="D93">
         <v>91287</v>
@@ -9145,19 +9166,19 @@
         <v>538</v>
       </c>
       <c r="F93" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="G93" t="s">
-        <v>551</v>
+        <v>27</v>
       </c>
       <c r="H93" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="I93" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="J93" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K93" t="s">
         <v>47</v>
@@ -9166,7 +9187,7 @@
         <v>40</v>
       </c>
       <c r="M93" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="N93" t="s">
         <v>30</v>
@@ -9175,25 +9196,25 @@
         <v>31</v>
       </c>
       <c r="P93" t="s">
-        <v>29</v>
+        <v>546</v>
       </c>
       <c r="Q93" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="R93" t="s">
-        <v>71</v>
+        <v>546</v>
       </c>
       <c r="S93" t="s">
-        <v>71</v>
+        <v>546</v>
       </c>
       <c r="T93" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="U93" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="V93" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="W93" t="s">
         <v>27</v>
@@ -9201,37 +9222,37 @@
     </row>
     <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="B94" t="s">
         <v>23</v>
       </c>
       <c r="C94" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="D94">
-        <v>91224</v>
+        <v>91287</v>
       </c>
       <c r="E94" t="s">
-        <v>556</v>
+        <v>538</v>
       </c>
       <c r="F94" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="G94" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="H94" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="I94" t="s">
         <v>29</v>
       </c>
       <c r="J94" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K94" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L94" t="s">
         <v>40</v>
@@ -9249,22 +9270,22 @@
         <v>29</v>
       </c>
       <c r="Q94" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="R94" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="S94" t="s">
-        <v>560</v>
+        <v>71</v>
       </c>
       <c r="T94" t="s">
-        <v>560</v>
+        <v>71</v>
       </c>
       <c r="U94" t="s">
-        <v>42</v>
+        <v>553</v>
       </c>
       <c r="V94" t="s">
-        <v>42</v>
+        <v>553</v>
       </c>
       <c r="W94" t="s">
         <v>27</v>
@@ -9272,13 +9293,13 @@
     </row>
     <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="B95" t="s">
         <v>23</v>
       </c>
       <c r="C95" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
       <c r="D95">
         <v>91224</v>
@@ -9287,25 +9308,25 @@
         <v>556</v>
       </c>
       <c r="F95" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="G95" t="s">
-        <v>27</v>
+        <v>558</v>
       </c>
       <c r="H95" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="I95" t="s">
         <v>29</v>
       </c>
       <c r="J95" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K95" t="s">
         <v>29</v>
       </c>
       <c r="L95" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="M95" t="s">
         <v>41</v>
@@ -9320,22 +9341,22 @@
         <v>29</v>
       </c>
       <c r="Q95" t="s">
-        <v>225</v>
+        <v>29</v>
       </c>
       <c r="R95" t="s">
         <v>29</v>
       </c>
       <c r="S95" t="s">
-        <v>29</v>
+        <v>560</v>
       </c>
       <c r="T95" t="s">
-        <v>225</v>
+        <v>560</v>
       </c>
       <c r="U95" t="s">
-        <v>401</v>
+        <v>42</v>
       </c>
       <c r="V95" t="s">
-        <v>565</v>
+        <v>42</v>
       </c>
       <c r="W95" t="s">
         <v>27</v>
@@ -9343,13 +9364,13 @@
     </row>
     <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="B96" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="C96" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="D96">
         <v>91224</v>
@@ -9358,13 +9379,13 @@
         <v>556</v>
       </c>
       <c r="F96" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="G96" t="s">
         <v>27</v>
       </c>
       <c r="H96" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="I96" t="s">
         <v>29</v>
@@ -9373,10 +9394,10 @@
         <v>39</v>
       </c>
       <c r="K96" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L96" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="M96" t="s">
         <v>41</v>
@@ -9391,22 +9412,22 @@
         <v>29</v>
       </c>
       <c r="Q96" t="s">
-        <v>106</v>
+        <v>225</v>
       </c>
       <c r="R96" t="s">
-        <v>106</v>
+        <v>29</v>
       </c>
       <c r="S96" t="s">
-        <v>106</v>
+        <v>29</v>
       </c>
       <c r="T96" t="s">
-        <v>106</v>
+        <v>225</v>
       </c>
       <c r="U96" t="s">
-        <v>106</v>
+        <v>401</v>
       </c>
       <c r="V96" t="s">
-        <v>106</v>
+        <v>565</v>
       </c>
       <c r="W96" t="s">
         <v>27</v>
@@ -9414,34 +9435,34 @@
     </row>
     <row r="97" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="B97" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="C97" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="D97">
-        <v>90552</v>
+        <v>91224</v>
       </c>
       <c r="E97" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="F97" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="G97" t="s">
-        <v>574</v>
+        <v>27</v>
       </c>
       <c r="H97" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="I97" t="s">
         <v>29</v>
       </c>
       <c r="J97" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K97" t="s">
         <v>47</v>
@@ -9462,22 +9483,22 @@
         <v>29</v>
       </c>
       <c r="Q97" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="R97" t="s">
-        <v>286</v>
+        <v>106</v>
       </c>
       <c r="S97" t="s">
-        <v>286</v>
+        <v>106</v>
       </c>
       <c r="T97" t="s">
-        <v>286</v>
+        <v>106</v>
       </c>
       <c r="U97" t="s">
-        <v>286</v>
+        <v>106</v>
       </c>
       <c r="V97" t="s">
-        <v>286</v>
+        <v>106</v>
       </c>
       <c r="W97" t="s">
         <v>27</v>
@@ -9485,13 +9506,13 @@
     </row>
     <row r="98" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="B98" t="s">
         <v>23</v>
       </c>
       <c r="C98" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="D98">
         <v>90552</v>
@@ -9500,13 +9521,13 @@
         <v>572</v>
       </c>
       <c r="F98" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="G98" t="s">
-        <v>27</v>
+        <v>574</v>
       </c>
       <c r="H98" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="I98" t="s">
         <v>29</v>
@@ -9536,19 +9557,19 @@
         <v>29</v>
       </c>
       <c r="R98" t="s">
-        <v>42</v>
+        <v>286</v>
       </c>
       <c r="S98" t="s">
-        <v>42</v>
+        <v>286</v>
       </c>
       <c r="T98" t="s">
-        <v>42</v>
+        <v>286</v>
       </c>
       <c r="U98" t="s">
-        <v>42</v>
+        <v>286</v>
       </c>
       <c r="V98" t="s">
-        <v>42</v>
+        <v>286</v>
       </c>
       <c r="W98" t="s">
         <v>27</v>
@@ -9556,13 +9577,13 @@
     </row>
     <row r="99" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="B99" t="s">
         <v>23</v>
       </c>
       <c r="C99" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="D99">
         <v>90552</v>
@@ -9571,22 +9592,22 @@
         <v>572</v>
       </c>
       <c r="F99" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="G99" t="s">
-        <v>583</v>
+        <v>27</v>
       </c>
       <c r="H99" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="I99" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J99" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K99" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L99" t="s">
         <v>40</v>
@@ -9601,25 +9622,25 @@
         <v>31</v>
       </c>
       <c r="P99" t="s">
-        <v>585</v>
+        <v>29</v>
       </c>
       <c r="Q99" t="s">
-        <v>585</v>
+        <v>29</v>
       </c>
       <c r="R99" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="S99" t="s">
-        <v>585</v>
+        <v>42</v>
       </c>
       <c r="T99" t="s">
-        <v>585</v>
+        <v>42</v>
       </c>
       <c r="U99" t="s">
-        <v>585</v>
+        <v>42</v>
       </c>
       <c r="V99" t="s">
-        <v>586</v>
+        <v>42</v>
       </c>
       <c r="W99" t="s">
         <v>27</v>
@@ -9627,37 +9648,37 @@
     </row>
     <row r="100" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
       <c r="B100" t="s">
         <v>23</v>
       </c>
       <c r="C100" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
       <c r="D100">
-        <v>91245</v>
+        <v>90552</v>
       </c>
       <c r="E100" t="s">
-        <v>589</v>
+        <v>572</v>
       </c>
       <c r="F100" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="G100" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
       <c r="H100" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="I100" t="s">
         <v>38</v>
       </c>
       <c r="J100" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K100" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L100" t="s">
         <v>40</v>
@@ -9672,25 +9693,25 @@
         <v>31</v>
       </c>
       <c r="P100" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="Q100" t="s">
-        <v>29</v>
+        <v>585</v>
       </c>
       <c r="R100" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="S100" t="s">
-        <v>42</v>
+        <v>585</v>
       </c>
       <c r="T100" t="s">
-        <v>42</v>
+        <v>585</v>
       </c>
       <c r="U100" t="s">
-        <v>594</v>
+        <v>585</v>
       </c>
       <c r="V100" t="s">
-        <v>595</v>
+        <v>586</v>
       </c>
       <c r="W100" t="s">
         <v>27</v>
@@ -9698,13 +9719,13 @@
     </row>
     <row r="101" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>596</v>
+        <v>587</v>
       </c>
       <c r="B101" t="s">
         <v>23</v>
       </c>
       <c r="C101" t="s">
-        <v>597</v>
+        <v>588</v>
       </c>
       <c r="D101">
         <v>91245</v>
@@ -9713,16 +9734,16 @@
         <v>589</v>
       </c>
       <c r="F101" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="G101" t="s">
-        <v>27</v>
+        <v>591</v>
       </c>
       <c r="H101" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
       <c r="I101" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="J101" t="s">
         <v>29</v>
@@ -9743,25 +9764,25 @@
         <v>31</v>
       </c>
       <c r="P101" t="s">
-        <v>29</v>
+        <v>593</v>
       </c>
       <c r="Q101" t="s">
         <v>29</v>
       </c>
       <c r="R101" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="S101" t="s">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="T101" t="s">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="U101" t="s">
-        <v>104</v>
+        <v>594</v>
       </c>
       <c r="V101" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="W101" t="s">
         <v>27</v>
@@ -9769,13 +9790,13 @@
     </row>
     <row r="102" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>647</v>
+        <v>596</v>
       </c>
       <c r="B102" t="s">
         <v>23</v>
       </c>
       <c r="C102" t="s">
-        <v>648</v>
+        <v>597</v>
       </c>
       <c r="D102">
         <v>91245</v>
@@ -9783,14 +9804,14 @@
       <c r="E102" t="s">
         <v>589</v>
       </c>
-      <c r="F102" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="G102" s="4" t="s">
-        <v>651</v>
-      </c>
-      <c r="H102" s="4" t="s">
-        <v>650</v>
+      <c r="F102" t="s">
+        <v>598</v>
+      </c>
+      <c r="G102" t="s">
+        <v>27</v>
+      </c>
+      <c r="H102" t="s">
+        <v>599</v>
       </c>
       <c r="I102" t="s">
         <v>29</v>
@@ -9820,19 +9841,19 @@
         <v>29</v>
       </c>
       <c r="R102" t="s">
-        <v>652</v>
+        <v>71</v>
       </c>
       <c r="S102" t="s">
-        <v>586</v>
+        <v>104</v>
       </c>
       <c r="T102" t="s">
-        <v>586</v>
+        <v>104</v>
       </c>
       <c r="U102" t="s">
-        <v>586</v>
+        <v>104</v>
       </c>
       <c r="V102" t="s">
-        <v>586</v>
+        <v>600</v>
       </c>
       <c r="W102" t="s">
         <v>27</v>
@@ -9840,28 +9861,28 @@
     </row>
     <row r="103" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>601</v>
+        <v>647</v>
       </c>
       <c r="B103" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="C103" t="s">
-        <v>602</v>
+        <v>648</v>
       </c>
       <c r="D103">
-        <v>91247</v>
+        <v>91245</v>
       </c>
       <c r="E103" t="s">
-        <v>603</v>
-      </c>
-      <c r="F103" t="s">
-        <v>604</v>
-      </c>
-      <c r="G103" t="s">
-        <v>27</v>
-      </c>
-      <c r="H103" t="s">
-        <v>605</v>
+        <v>589</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="G103" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="H103" s="4" t="s">
+        <v>650</v>
       </c>
       <c r="I103" t="s">
         <v>29</v>
@@ -9870,13 +9891,13 @@
         <v>29</v>
       </c>
       <c r="K103" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L103" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="M103" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="N103" t="s">
         <v>30</v>
@@ -9891,19 +9912,19 @@
         <v>29</v>
       </c>
       <c r="R103" t="s">
-        <v>29</v>
+        <v>652</v>
       </c>
       <c r="S103" t="s">
-        <v>29</v>
+        <v>586</v>
       </c>
       <c r="T103" t="s">
-        <v>29</v>
+        <v>586</v>
       </c>
       <c r="U103" t="s">
-        <v>72</v>
+        <v>586</v>
       </c>
       <c r="V103" t="s">
-        <v>606</v>
+        <v>586</v>
       </c>
       <c r="W103" t="s">
         <v>27</v>
@@ -9911,13 +9932,13 @@
     </row>
     <row r="104" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="B104" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C104" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="D104">
         <v>91247</v>
@@ -9926,28 +9947,28 @@
         <v>603</v>
       </c>
       <c r="F104" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="G104" t="s">
-        <v>610</v>
+        <v>27</v>
       </c>
       <c r="H104" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="I104" t="s">
         <v>29</v>
       </c>
       <c r="J104" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K104" t="s">
         <v>29</v>
       </c>
       <c r="L104" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="M104" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="N104" t="s">
         <v>30</v>
@@ -9959,22 +9980,22 @@
         <v>29</v>
       </c>
       <c r="Q104" t="s">
-        <v>612</v>
+        <v>29</v>
       </c>
       <c r="R104" t="s">
         <v>29</v>
       </c>
       <c r="S104" t="s">
-        <v>612</v>
+        <v>29</v>
       </c>
       <c r="T104" t="s">
-        <v>612</v>
+        <v>29</v>
       </c>
       <c r="U104" t="s">
-        <v>612</v>
+        <v>72</v>
       </c>
       <c r="V104" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="W104" t="s">
         <v>27</v>
@@ -9982,13 +10003,13 @@
     </row>
     <row r="105" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="B105" t="s">
         <v>23</v>
       </c>
       <c r="C105" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="D105">
         <v>91247</v>
@@ -9997,25 +10018,25 @@
         <v>603</v>
       </c>
       <c r="F105" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="G105" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="H105" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="I105" t="s">
         <v>29</v>
       </c>
       <c r="J105" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K105" t="s">
         <v>29</v>
       </c>
       <c r="L105" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="M105" t="s">
         <v>41</v>
@@ -10030,22 +10051,22 @@
         <v>29</v>
       </c>
       <c r="Q105" t="s">
-        <v>29</v>
+        <v>612</v>
       </c>
       <c r="R105" t="s">
         <v>29</v>
       </c>
       <c r="S105" t="s">
-        <v>29</v>
+        <v>612</v>
       </c>
       <c r="T105" t="s">
-        <v>469</v>
+        <v>612</v>
       </c>
       <c r="U105" t="s">
-        <v>469</v>
+        <v>612</v>
       </c>
       <c r="V105" t="s">
-        <v>57</v>
+        <v>612</v>
       </c>
       <c r="W105" t="s">
         <v>27</v>
@@ -10053,28 +10074,28 @@
     </row>
     <row r="106" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="B106" t="s">
         <v>23</v>
       </c>
       <c r="C106" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="D106">
-        <v>91367</v>
+        <v>91247</v>
       </c>
       <c r="E106" t="s">
-        <v>620</v>
+        <v>603</v>
       </c>
       <c r="F106" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="G106" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="H106" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="I106" t="s">
         <v>29</v>
@@ -10086,7 +10107,7 @@
         <v>29</v>
       </c>
       <c r="L106" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="M106" t="s">
         <v>41</v>
@@ -10107,16 +10128,16 @@
         <v>29</v>
       </c>
       <c r="S106" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="T106" t="s">
-        <v>72</v>
+        <v>469</v>
       </c>
       <c r="U106" t="s">
-        <v>72</v>
+        <v>469</v>
       </c>
       <c r="V106" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="W106" t="s">
         <v>27</v>
@@ -10124,13 +10145,13 @@
     </row>
     <row r="107" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="B107" t="s">
         <v>23</v>
       </c>
       <c r="C107" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="D107">
         <v>91367</v>
@@ -10139,22 +10160,22 @@
         <v>620</v>
       </c>
       <c r="F107" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="G107" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="H107" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="I107" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J107" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K107" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L107" t="s">
         <v>40</v>
@@ -10166,30 +10187,101 @@
         <v>30</v>
       </c>
       <c r="O107" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P107" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q107" t="s">
+        <v>29</v>
+      </c>
+      <c r="R107" t="s">
+        <v>29</v>
+      </c>
+      <c r="S107" t="s">
+        <v>71</v>
+      </c>
+      <c r="T107" t="s">
+        <v>72</v>
+      </c>
+      <c r="U107" t="s">
+        <v>72</v>
+      </c>
+      <c r="V107" t="s">
+        <v>72</v>
+      </c>
+      <c r="W107" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>624</v>
+      </c>
+      <c r="B108" t="s">
+        <v>23</v>
+      </c>
+      <c r="C108" t="s">
+        <v>625</v>
+      </c>
+      <c r="D108">
+        <v>91367</v>
+      </c>
+      <c r="E108" t="s">
+        <v>620</v>
+      </c>
+      <c r="F108" t="s">
+        <v>626</v>
+      </c>
+      <c r="G108" t="s">
+        <v>627</v>
+      </c>
+      <c r="H108" t="s">
+        <v>628</v>
+      </c>
+      <c r="I108" t="s">
+        <v>38</v>
+      </c>
+      <c r="J108" t="s">
+        <v>39</v>
+      </c>
+      <c r="K108" t="s">
+        <v>47</v>
+      </c>
+      <c r="L108" t="s">
+        <v>40</v>
+      </c>
+      <c r="M108" t="s">
+        <v>41</v>
+      </c>
+      <c r="N108" t="s">
+        <v>30</v>
+      </c>
+      <c r="O108" t="s">
+        <v>29</v>
+      </c>
+      <c r="P108" t="s">
         <v>629</v>
       </c>
-      <c r="Q107" t="s">
+      <c r="Q108" t="s">
         <v>629</v>
       </c>
-      <c r="R107" t="s">
+      <c r="R108" t="s">
         <v>629</v>
       </c>
-      <c r="S107" t="s">
+      <c r="S108" t="s">
         <v>629</v>
       </c>
-      <c r="T107" t="s">
+      <c r="T108" t="s">
         <v>629</v>
       </c>
-      <c r="U107" t="s">
+      <c r="U108" t="s">
         <v>630</v>
       </c>
-      <c r="V107" t="s">
-        <v>29</v>
-      </c>
-      <c r="W107" t="s">
+      <c r="V108" t="s">
+        <v>29</v>
+      </c>
+      <c r="W108" t="s">
         <v>27</v>
       </c>
     </row>
@@ -10197,18 +10289,19 @@
   <hyperlinks>
     <hyperlink ref="H58" r:id="rId1" xr:uid="{3518E2E3-45F1-448A-93F8-FA096D84A577}"/>
     <hyperlink ref="G58" r:id="rId2" xr:uid="{7220F707-B88F-4FDE-AEBA-ED4F716E05CE}"/>
-    <hyperlink ref="H81" r:id="rId3" xr:uid="{AD9CFEB0-515E-47DE-A619-8A0566327566}"/>
+    <hyperlink ref="H82" r:id="rId3" xr:uid="{AD9CFEB0-515E-47DE-A619-8A0566327566}"/>
     <hyperlink ref="G68" r:id="rId4" xr:uid="{C5402745-E279-4144-A7EA-01FCE7A4E404}"/>
     <hyperlink ref="H68" r:id="rId5" xr:uid="{679F818E-03B4-4BF2-B47A-7E4540C537AF}"/>
-    <hyperlink ref="H102" r:id="rId6" xr:uid="{64B05FEF-865E-4E04-B288-9B0F0E91EB19}"/>
-    <hyperlink ref="G102" r:id="rId7" xr:uid="{1C619C93-40F6-455D-B3C4-D8F5DA0E79E2}"/>
+    <hyperlink ref="H103" r:id="rId6" xr:uid="{64B05FEF-865E-4E04-B288-9B0F0E91EB19}"/>
+    <hyperlink ref="G103" r:id="rId7" xr:uid="{1C619C93-40F6-455D-B3C4-D8F5DA0E79E2}"/>
     <hyperlink ref="H66" r:id="rId8" xr:uid="{811F14D2-8625-407A-A363-4868792D85E3}"/>
     <hyperlink ref="G73" r:id="rId9" xr:uid="{91676D4A-98DC-43A6-8746-157BFB405308}"/>
     <hyperlink ref="H73" r:id="rId10" xr:uid="{03594D0E-5B3F-4FCC-9030-CF67D477ED14}"/>
+    <hyperlink ref="H79" r:id="rId11" xr:uid="{9348353F-C4D8-4830-99C4-699BA05B7D2C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
URL of schlosskellrer corrected
</commit_message>
<xml_diff>
--- a/cfg/pubfinder_list_NLA.xlsx
+++ b/cfg/pubfinder_list_NLA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_dev\pubfinder_V2\cfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9578AE34-1123-43CC-9D2B-5A4FF8251A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085B75CF-7387-4648-929D-DE0B1A2DF75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{75E81789-C525-4005-96BA-B080353C5F6C}"/>
   </bookViews>
@@ -2057,13 +2057,13 @@
     <t>+499123966635</t>
   </si>
   <si>
-    <t>www.schlosskeller-lauf.de</t>
-  </si>
-  <si>
     <t>18:00 - 01:00</t>
   </si>
   <si>
     <t>18:00 - 03:00</t>
+  </si>
+  <si>
+    <t>http://www.schlosskeller-lauf.de</t>
   </si>
 </sst>
 </file>
@@ -2593,8 +2593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F2D7F2-8E23-4C59-B8E8-2949683E6C83}">
   <dimension ref="A1:W108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I64" workbookViewId="0">
-      <selection activeCell="T79" sqref="T79"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="H79" sqref="H79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8178,7 +8178,7 @@
         <v>27</v>
       </c>
       <c r="H79" s="4" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="I79" t="s">
         <v>29</v>
@@ -8211,16 +8211,16 @@
         <v>29</v>
       </c>
       <c r="S79" t="s">
+        <v>669</v>
+      </c>
+      <c r="T79" t="s">
         <v>670</v>
       </c>
-      <c r="T79" t="s">
-        <v>671</v>
-      </c>
       <c r="U79" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="V79" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="W79" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Rhodos in Leinburg added
</commit_message>
<xml_diff>
--- a/cfg/pubfinder_list_NLA.xlsx
+++ b/cfg/pubfinder_list_NLA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_dev\pubfinder_V2\cfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085B75CF-7387-4648-929D-DE0B1A2DF75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB1269C-FD33-4281-B934-E851A4D8501C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{75E81789-C525-4005-96BA-B080353C5F6C}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">pubfinder_list_NLA!$A$1:$W$108</definedName>
+    <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">pubfinder_list_NLA!$A$1:$W$109</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2376" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2397" uniqueCount="677">
   <si>
     <t>Name</t>
   </si>
@@ -2064,6 +2064,21 @@
   </si>
   <si>
     <t>http://www.schlosskeller-lauf.de</t>
+  </si>
+  <si>
+    <t>Rhodos</t>
+  </si>
+  <si>
+    <t>+4991204719922</t>
+  </si>
+  <si>
+    <t>https://rhodos-leinburg.de/</t>
+  </si>
+  <si>
+    <t>17:00 - 23:30</t>
+  </si>
+  <si>
+    <t>11:00 - 14:00 &amp; 17:00 - 23:30</t>
   </si>
 </sst>
 </file>
@@ -2243,8 +2258,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C4BF8B3-CB62-48F7-AAC2-6E12CB367C86}" name="pubfinder_list_NLA_ok" displayName="pubfinder_list_NLA_ok" ref="A1:W108" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:W108" xr:uid="{1C4BF8B3-CB62-48F7-AAC2-6E12CB367C86}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C4BF8B3-CB62-48F7-AAC2-6E12CB367C86}" name="pubfinder_list_NLA_ok" displayName="pubfinder_list_NLA_ok" ref="A1:W109" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:W109" xr:uid="{1C4BF8B3-CB62-48F7-AAC2-6E12CB367C86}"/>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{92103B2C-FCC3-42D2-95DB-A3F77D77EC29}" uniqueName="1" name="Name" queryTableFieldId="1" dataDxfId="21"/>
     <tableColumn id="2" xr3:uid="{86208C35-2046-4F53-B583-F5FD55ED84C8}" uniqueName="2" name="Typ" queryTableFieldId="2" dataDxfId="20"/>
@@ -2591,10 +2606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F2D7F2-8E23-4C59-B8E8-2949683E6C83}">
-  <dimension ref="A1:W108"/>
+  <dimension ref="A1:W109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="H79" sqref="H79"/>
+    <sheetView tabSelected="1" topLeftCell="J64" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88:XFD88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8796,40 +8811,37 @@
     </row>
     <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>511</v>
+        <v>672</v>
       </c>
       <c r="B88" t="s">
-        <v>23</v>
+        <v>249</v>
       </c>
       <c r="C88" t="s">
-        <v>512</v>
+        <v>537</v>
       </c>
       <c r="D88">
-        <v>91284</v>
+        <v>91227</v>
       </c>
       <c r="E88" t="s">
-        <v>513</v>
-      </c>
-      <c r="F88" t="s">
-        <v>514</v>
-      </c>
-      <c r="G88" t="s">
-        <v>515</v>
-      </c>
-      <c r="H88" t="s">
-        <v>516</v>
+        <v>493</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>674</v>
       </c>
       <c r="I88" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="J88" t="s">
         <v>29</v>
       </c>
       <c r="K88" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L88" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="M88" t="s">
         <v>41</v>
@@ -8841,25 +8853,25 @@
         <v>31</v>
       </c>
       <c r="P88" t="s">
-        <v>29</v>
+        <v>675</v>
       </c>
       <c r="Q88" t="s">
         <v>29</v>
       </c>
       <c r="R88" t="s">
-        <v>29</v>
+        <v>675</v>
       </c>
       <c r="S88" t="s">
-        <v>29</v>
+        <v>675</v>
       </c>
       <c r="T88" t="s">
-        <v>56</v>
+        <v>675</v>
       </c>
       <c r="U88" t="s">
-        <v>163</v>
+        <v>675</v>
       </c>
       <c r="V88" t="s">
-        <v>163</v>
+        <v>676</v>
       </c>
       <c r="W88" t="s">
         <v>27</v>
@@ -8867,28 +8879,28 @@
     </row>
     <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="B89" t="s">
         <v>23</v>
       </c>
       <c r="C89" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="D89">
-        <v>91233</v>
+        <v>91284</v>
       </c>
       <c r="E89" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="F89" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="G89" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="H89" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="I89" t="s">
         <v>29</v>
@@ -8906,7 +8918,7 @@
         <v>41</v>
       </c>
       <c r="N89" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O89" t="s">
         <v>31</v>
@@ -8924,13 +8936,13 @@
         <v>29</v>
       </c>
       <c r="T89" t="s">
-        <v>523</v>
+        <v>56</v>
       </c>
       <c r="U89" t="s">
-        <v>29</v>
+        <v>163</v>
       </c>
       <c r="V89" t="s">
-        <v>524</v>
+        <v>163</v>
       </c>
       <c r="W89" t="s">
         <v>27</v>
@@ -8938,46 +8950,46 @@
     </row>
     <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="B90" t="s">
-        <v>249</v>
+        <v>23</v>
       </c>
       <c r="C90" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="D90">
-        <v>91242</v>
+        <v>91233</v>
       </c>
       <c r="E90" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="F90" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="G90" t="s">
-        <v>27</v>
+        <v>521</v>
       </c>
       <c r="H90" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="I90" t="s">
         <v>29</v>
       </c>
       <c r="J90" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K90" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L90" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="M90" t="s">
         <v>41</v>
       </c>
       <c r="N90" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O90" t="s">
         <v>31</v>
@@ -8986,22 +8998,22 @@
         <v>29</v>
       </c>
       <c r="Q90" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="R90" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="S90" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="T90" t="s">
-        <v>71</v>
+        <v>523</v>
       </c>
       <c r="U90" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="V90" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="W90" t="s">
         <v>27</v>
@@ -9009,13 +9021,13 @@
     </row>
     <row r="91" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="B91" t="s">
-        <v>23</v>
+        <v>249</v>
       </c>
       <c r="C91" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="D91">
         <v>91242</v>
@@ -9024,19 +9036,19 @@
         <v>527</v>
       </c>
       <c r="F91" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="G91" t="s">
         <v>27</v>
       </c>
       <c r="H91" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="I91" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J91" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K91" t="s">
         <v>47</v>
@@ -9054,25 +9066,25 @@
         <v>31</v>
       </c>
       <c r="P91" t="s">
-        <v>535</v>
+        <v>29</v>
       </c>
       <c r="Q91" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="R91" t="s">
-        <v>535</v>
+        <v>71</v>
       </c>
       <c r="S91" t="s">
-        <v>535</v>
+        <v>71</v>
       </c>
       <c r="T91" t="s">
-        <v>234</v>
+        <v>71</v>
       </c>
       <c r="U91" t="s">
-        <v>234</v>
+        <v>71</v>
       </c>
       <c r="V91" t="s">
-        <v>234</v>
+        <v>530</v>
       </c>
       <c r="W91" t="s">
         <v>27</v>
@@ -9080,37 +9092,37 @@
     </row>
     <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="B92" t="s">
         <v>23</v>
       </c>
       <c r="C92" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D92">
-        <v>91287</v>
+        <v>91242</v>
       </c>
       <c r="E92" t="s">
-        <v>538</v>
+        <v>527</v>
       </c>
       <c r="F92" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="G92" t="s">
-        <v>540</v>
+        <v>27</v>
       </c>
       <c r="H92" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="I92" t="s">
         <v>38</v>
       </c>
       <c r="J92" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K92" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L92" t="s">
         <v>40</v>
@@ -9125,25 +9137,25 @@
         <v>31</v>
       </c>
       <c r="P92" t="s">
-        <v>292</v>
+        <v>535</v>
       </c>
       <c r="Q92" t="s">
-        <v>292</v>
+        <v>29</v>
       </c>
       <c r="R92" t="s">
-        <v>29</v>
+        <v>535</v>
       </c>
       <c r="S92" t="s">
-        <v>292</v>
+        <v>535</v>
       </c>
       <c r="T92" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
       <c r="U92" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
       <c r="V92" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
       <c r="W92" t="s">
         <v>27</v>
@@ -9151,13 +9163,13 @@
     </row>
     <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="B93" t="s">
         <v>23</v>
       </c>
       <c r="C93" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="D93">
         <v>91287</v>
@@ -9166,28 +9178,28 @@
         <v>538</v>
       </c>
       <c r="F93" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="G93" t="s">
-        <v>27</v>
+        <v>540</v>
       </c>
       <c r="H93" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="I93" t="s">
         <v>38</v>
       </c>
       <c r="J93" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K93" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L93" t="s">
         <v>40</v>
       </c>
       <c r="M93" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="N93" t="s">
         <v>30</v>
@@ -9196,25 +9208,25 @@
         <v>31</v>
       </c>
       <c r="P93" t="s">
-        <v>546</v>
+        <v>292</v>
       </c>
       <c r="Q93" t="s">
-        <v>29</v>
+        <v>292</v>
       </c>
       <c r="R93" t="s">
-        <v>546</v>
+        <v>29</v>
       </c>
       <c r="S93" t="s">
-        <v>546</v>
+        <v>292</v>
       </c>
       <c r="T93" t="s">
-        <v>29</v>
+        <v>292</v>
       </c>
       <c r="U93" t="s">
-        <v>546</v>
+        <v>292</v>
       </c>
       <c r="V93" t="s">
-        <v>547</v>
+        <v>292</v>
       </c>
       <c r="W93" t="s">
         <v>27</v>
@@ -9222,13 +9234,13 @@
     </row>
     <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="B94" t="s">
         <v>23</v>
       </c>
       <c r="C94" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="D94">
         <v>91287</v>
@@ -9237,19 +9249,19 @@
         <v>538</v>
       </c>
       <c r="F94" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="G94" t="s">
-        <v>551</v>
+        <v>27</v>
       </c>
       <c r="H94" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="I94" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="J94" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K94" t="s">
         <v>47</v>
@@ -9258,7 +9270,7 @@
         <v>40</v>
       </c>
       <c r="M94" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="N94" t="s">
         <v>30</v>
@@ -9267,25 +9279,25 @@
         <v>31</v>
       </c>
       <c r="P94" t="s">
-        <v>29</v>
+        <v>546</v>
       </c>
       <c r="Q94" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="R94" t="s">
-        <v>71</v>
+        <v>546</v>
       </c>
       <c r="S94" t="s">
-        <v>71</v>
+        <v>546</v>
       </c>
       <c r="T94" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="U94" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="V94" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="W94" t="s">
         <v>27</v>
@@ -9293,37 +9305,37 @@
     </row>
     <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="B95" t="s">
         <v>23</v>
       </c>
       <c r="C95" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="D95">
-        <v>91224</v>
+        <v>91287</v>
       </c>
       <c r="E95" t="s">
-        <v>556</v>
+        <v>538</v>
       </c>
       <c r="F95" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="G95" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="H95" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="I95" t="s">
         <v>29</v>
       </c>
       <c r="J95" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K95" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L95" t="s">
         <v>40</v>
@@ -9341,22 +9353,22 @@
         <v>29</v>
       </c>
       <c r="Q95" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="R95" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="S95" t="s">
-        <v>560</v>
+        <v>71</v>
       </c>
       <c r="T95" t="s">
-        <v>560</v>
+        <v>71</v>
       </c>
       <c r="U95" t="s">
-        <v>42</v>
+        <v>553</v>
       </c>
       <c r="V95" t="s">
-        <v>42</v>
+        <v>553</v>
       </c>
       <c r="W95" t="s">
         <v>27</v>
@@ -9364,13 +9376,13 @@
     </row>
     <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="B96" t="s">
         <v>23</v>
       </c>
       <c r="C96" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
       <c r="D96">
         <v>91224</v>
@@ -9379,25 +9391,25 @@
         <v>556</v>
       </c>
       <c r="F96" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="G96" t="s">
-        <v>27</v>
+        <v>558</v>
       </c>
       <c r="H96" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="I96" t="s">
         <v>29</v>
       </c>
       <c r="J96" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K96" t="s">
         <v>29</v>
       </c>
       <c r="L96" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="M96" t="s">
         <v>41</v>
@@ -9412,22 +9424,22 @@
         <v>29</v>
       </c>
       <c r="Q96" t="s">
-        <v>225</v>
+        <v>29</v>
       </c>
       <c r="R96" t="s">
         <v>29</v>
       </c>
       <c r="S96" t="s">
-        <v>29</v>
+        <v>560</v>
       </c>
       <c r="T96" t="s">
-        <v>225</v>
+        <v>560</v>
       </c>
       <c r="U96" t="s">
-        <v>401</v>
+        <v>42</v>
       </c>
       <c r="V96" t="s">
-        <v>565</v>
+        <v>42</v>
       </c>
       <c r="W96" t="s">
         <v>27</v>
@@ -9435,13 +9447,13 @@
     </row>
     <row r="97" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="B97" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="C97" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="D97">
         <v>91224</v>
@@ -9450,13 +9462,13 @@
         <v>556</v>
       </c>
       <c r="F97" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="G97" t="s">
         <v>27</v>
       </c>
       <c r="H97" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="I97" t="s">
         <v>29</v>
@@ -9465,10 +9477,10 @@
         <v>39</v>
       </c>
       <c r="K97" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L97" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="M97" t="s">
         <v>41</v>
@@ -9483,22 +9495,22 @@
         <v>29</v>
       </c>
       <c r="Q97" t="s">
-        <v>106</v>
+        <v>225</v>
       </c>
       <c r="R97" t="s">
-        <v>106</v>
+        <v>29</v>
       </c>
       <c r="S97" t="s">
-        <v>106</v>
+        <v>29</v>
       </c>
       <c r="T97" t="s">
-        <v>106</v>
+        <v>225</v>
       </c>
       <c r="U97" t="s">
-        <v>106</v>
+        <v>401</v>
       </c>
       <c r="V97" t="s">
-        <v>106</v>
+        <v>565</v>
       </c>
       <c r="W97" t="s">
         <v>27</v>
@@ -9506,34 +9518,34 @@
     </row>
     <row r="98" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="B98" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="C98" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="D98">
-        <v>90552</v>
+        <v>91224</v>
       </c>
       <c r="E98" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="F98" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="G98" t="s">
-        <v>574</v>
+        <v>27</v>
       </c>
       <c r="H98" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="I98" t="s">
         <v>29</v>
       </c>
       <c r="J98" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K98" t="s">
         <v>47</v>
@@ -9554,22 +9566,22 @@
         <v>29</v>
       </c>
       <c r="Q98" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="R98" t="s">
-        <v>286</v>
+        <v>106</v>
       </c>
       <c r="S98" t="s">
-        <v>286</v>
+        <v>106</v>
       </c>
       <c r="T98" t="s">
-        <v>286</v>
+        <v>106</v>
       </c>
       <c r="U98" t="s">
-        <v>286</v>
+        <v>106</v>
       </c>
       <c r="V98" t="s">
-        <v>286</v>
+        <v>106</v>
       </c>
       <c r="W98" t="s">
         <v>27</v>
@@ -9577,13 +9589,13 @@
     </row>
     <row r="99" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="B99" t="s">
         <v>23</v>
       </c>
       <c r="C99" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="D99">
         <v>90552</v>
@@ -9592,13 +9604,13 @@
         <v>572</v>
       </c>
       <c r="F99" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="G99" t="s">
-        <v>27</v>
+        <v>574</v>
       </c>
       <c r="H99" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="I99" t="s">
         <v>29</v>
@@ -9628,19 +9640,19 @@
         <v>29</v>
       </c>
       <c r="R99" t="s">
-        <v>42</v>
+        <v>286</v>
       </c>
       <c r="S99" t="s">
-        <v>42</v>
+        <v>286</v>
       </c>
       <c r="T99" t="s">
-        <v>42</v>
+        <v>286</v>
       </c>
       <c r="U99" t="s">
-        <v>42</v>
+        <v>286</v>
       </c>
       <c r="V99" t="s">
-        <v>42</v>
+        <v>286</v>
       </c>
       <c r="W99" t="s">
         <v>27</v>
@@ -9648,13 +9660,13 @@
     </row>
     <row r="100" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="B100" t="s">
         <v>23</v>
       </c>
       <c r="C100" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="D100">
         <v>90552</v>
@@ -9663,22 +9675,22 @@
         <v>572</v>
       </c>
       <c r="F100" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="G100" t="s">
-        <v>583</v>
+        <v>27</v>
       </c>
       <c r="H100" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="I100" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J100" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K100" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L100" t="s">
         <v>40</v>
@@ -9693,25 +9705,25 @@
         <v>31</v>
       </c>
       <c r="P100" t="s">
-        <v>585</v>
+        <v>29</v>
       </c>
       <c r="Q100" t="s">
-        <v>585</v>
+        <v>29</v>
       </c>
       <c r="R100" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="S100" t="s">
-        <v>585</v>
+        <v>42</v>
       </c>
       <c r="T100" t="s">
-        <v>585</v>
+        <v>42</v>
       </c>
       <c r="U100" t="s">
-        <v>585</v>
+        <v>42</v>
       </c>
       <c r="V100" t="s">
-        <v>586</v>
+        <v>42</v>
       </c>
       <c r="W100" t="s">
         <v>27</v>
@@ -9719,37 +9731,37 @@
     </row>
     <row r="101" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
       <c r="B101" t="s">
         <v>23</v>
       </c>
       <c r="C101" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
       <c r="D101">
-        <v>91245</v>
+        <v>90552</v>
       </c>
       <c r="E101" t="s">
-        <v>589</v>
+        <v>572</v>
       </c>
       <c r="F101" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="G101" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
       <c r="H101" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="I101" t="s">
         <v>38</v>
       </c>
       <c r="J101" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K101" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L101" t="s">
         <v>40</v>
@@ -9764,25 +9776,25 @@
         <v>31</v>
       </c>
       <c r="P101" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="Q101" t="s">
-        <v>29</v>
+        <v>585</v>
       </c>
       <c r="R101" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="S101" t="s">
-        <v>42</v>
+        <v>585</v>
       </c>
       <c r="T101" t="s">
-        <v>42</v>
+        <v>585</v>
       </c>
       <c r="U101" t="s">
-        <v>594</v>
+        <v>585</v>
       </c>
       <c r="V101" t="s">
-        <v>595</v>
+        <v>586</v>
       </c>
       <c r="W101" t="s">
         <v>27</v>
@@ -9790,13 +9802,13 @@
     </row>
     <row r="102" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>596</v>
+        <v>587</v>
       </c>
       <c r="B102" t="s">
         <v>23</v>
       </c>
       <c r="C102" t="s">
-        <v>597</v>
+        <v>588</v>
       </c>
       <c r="D102">
         <v>91245</v>
@@ -9805,16 +9817,16 @@
         <v>589</v>
       </c>
       <c r="F102" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="G102" t="s">
-        <v>27</v>
+        <v>591</v>
       </c>
       <c r="H102" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
       <c r="I102" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="J102" t="s">
         <v>29</v>
@@ -9835,25 +9847,25 @@
         <v>31</v>
       </c>
       <c r="P102" t="s">
-        <v>29</v>
+        <v>593</v>
       </c>
       <c r="Q102" t="s">
         <v>29</v>
       </c>
       <c r="R102" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="S102" t="s">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="T102" t="s">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="U102" t="s">
-        <v>104</v>
+        <v>594</v>
       </c>
       <c r="V102" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="W102" t="s">
         <v>27</v>
@@ -9861,13 +9873,13 @@
     </row>
     <row r="103" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>647</v>
+        <v>596</v>
       </c>
       <c r="B103" t="s">
         <v>23</v>
       </c>
       <c r="C103" t="s">
-        <v>648</v>
+        <v>597</v>
       </c>
       <c r="D103">
         <v>91245</v>
@@ -9875,14 +9887,14 @@
       <c r="E103" t="s">
         <v>589</v>
       </c>
-      <c r="F103" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="G103" s="4" t="s">
-        <v>651</v>
-      </c>
-      <c r="H103" s="4" t="s">
-        <v>650</v>
+      <c r="F103" t="s">
+        <v>598</v>
+      </c>
+      <c r="G103" t="s">
+        <v>27</v>
+      </c>
+      <c r="H103" t="s">
+        <v>599</v>
       </c>
       <c r="I103" t="s">
         <v>29</v>
@@ -9912,19 +9924,19 @@
         <v>29</v>
       </c>
       <c r="R103" t="s">
-        <v>652</v>
+        <v>71</v>
       </c>
       <c r="S103" t="s">
-        <v>586</v>
+        <v>104</v>
       </c>
       <c r="T103" t="s">
-        <v>586</v>
+        <v>104</v>
       </c>
       <c r="U103" t="s">
-        <v>586</v>
+        <v>104</v>
       </c>
       <c r="V103" t="s">
-        <v>586</v>
+        <v>600</v>
       </c>
       <c r="W103" t="s">
         <v>27</v>
@@ -9932,28 +9944,28 @@
     </row>
     <row r="104" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>601</v>
+        <v>647</v>
       </c>
       <c r="B104" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="C104" t="s">
-        <v>602</v>
+        <v>648</v>
       </c>
       <c r="D104">
-        <v>91247</v>
+        <v>91245</v>
       </c>
       <c r="E104" t="s">
-        <v>603</v>
-      </c>
-      <c r="F104" t="s">
-        <v>604</v>
-      </c>
-      <c r="G104" t="s">
-        <v>27</v>
-      </c>
-      <c r="H104" t="s">
-        <v>605</v>
+        <v>589</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="G104" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="H104" s="4" t="s">
+        <v>650</v>
       </c>
       <c r="I104" t="s">
         <v>29</v>
@@ -9962,13 +9974,13 @@
         <v>29</v>
       </c>
       <c r="K104" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L104" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="M104" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="N104" t="s">
         <v>30</v>
@@ -9983,19 +9995,19 @@
         <v>29</v>
       </c>
       <c r="R104" t="s">
-        <v>29</v>
+        <v>652</v>
       </c>
       <c r="S104" t="s">
-        <v>29</v>
+        <v>586</v>
       </c>
       <c r="T104" t="s">
-        <v>29</v>
+        <v>586</v>
       </c>
       <c r="U104" t="s">
-        <v>72</v>
+        <v>586</v>
       </c>
       <c r="V104" t="s">
-        <v>606</v>
+        <v>586</v>
       </c>
       <c r="W104" t="s">
         <v>27</v>
@@ -10003,13 +10015,13 @@
     </row>
     <row r="105" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="B105" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C105" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="D105">
         <v>91247</v>
@@ -10018,28 +10030,28 @@
         <v>603</v>
       </c>
       <c r="F105" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="G105" t="s">
-        <v>610</v>
+        <v>27</v>
       </c>
       <c r="H105" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="I105" t="s">
         <v>29</v>
       </c>
       <c r="J105" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K105" t="s">
         <v>29</v>
       </c>
       <c r="L105" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="M105" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="N105" t="s">
         <v>30</v>
@@ -10051,22 +10063,22 @@
         <v>29</v>
       </c>
       <c r="Q105" t="s">
-        <v>612</v>
+        <v>29</v>
       </c>
       <c r="R105" t="s">
         <v>29</v>
       </c>
       <c r="S105" t="s">
-        <v>612</v>
+        <v>29</v>
       </c>
       <c r="T105" t="s">
-        <v>612</v>
+        <v>29</v>
       </c>
       <c r="U105" t="s">
-        <v>612</v>
+        <v>72</v>
       </c>
       <c r="V105" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="W105" t="s">
         <v>27</v>
@@ -10074,13 +10086,13 @@
     </row>
     <row r="106" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="B106" t="s">
         <v>23</v>
       </c>
       <c r="C106" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="D106">
         <v>91247</v>
@@ -10089,25 +10101,25 @@
         <v>603</v>
       </c>
       <c r="F106" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="G106" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="H106" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="I106" t="s">
         <v>29</v>
       </c>
       <c r="J106" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K106" t="s">
         <v>29</v>
       </c>
       <c r="L106" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="M106" t="s">
         <v>41</v>
@@ -10122,22 +10134,22 @@
         <v>29</v>
       </c>
       <c r="Q106" t="s">
-        <v>29</v>
+        <v>612</v>
       </c>
       <c r="R106" t="s">
         <v>29</v>
       </c>
       <c r="S106" t="s">
-        <v>29</v>
+        <v>612</v>
       </c>
       <c r="T106" t="s">
-        <v>469</v>
+        <v>612</v>
       </c>
       <c r="U106" t="s">
-        <v>469</v>
+        <v>612</v>
       </c>
       <c r="V106" t="s">
-        <v>57</v>
+        <v>612</v>
       </c>
       <c r="W106" t="s">
         <v>27</v>
@@ -10145,28 +10157,28 @@
     </row>
     <row r="107" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="B107" t="s">
         <v>23</v>
       </c>
       <c r="C107" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="D107">
-        <v>91367</v>
+        <v>91247</v>
       </c>
       <c r="E107" t="s">
-        <v>620</v>
+        <v>603</v>
       </c>
       <c r="F107" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="G107" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="H107" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="I107" t="s">
         <v>29</v>
@@ -10178,7 +10190,7 @@
         <v>29</v>
       </c>
       <c r="L107" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="M107" t="s">
         <v>41</v>
@@ -10199,16 +10211,16 @@
         <v>29</v>
       </c>
       <c r="S107" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="T107" t="s">
-        <v>72</v>
+        <v>469</v>
       </c>
       <c r="U107" t="s">
-        <v>72</v>
+        <v>469</v>
       </c>
       <c r="V107" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="W107" t="s">
         <v>27</v>
@@ -10216,13 +10228,13 @@
     </row>
     <row r="108" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="B108" t="s">
         <v>23</v>
       </c>
       <c r="C108" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="D108">
         <v>91367</v>
@@ -10231,22 +10243,22 @@
         <v>620</v>
       </c>
       <c r="F108" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="G108" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="H108" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="I108" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="J108" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K108" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="L108" t="s">
         <v>40</v>
@@ -10258,30 +10270,101 @@
         <v>30</v>
       </c>
       <c r="O108" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P108" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q108" t="s">
+        <v>29</v>
+      </c>
+      <c r="R108" t="s">
+        <v>29</v>
+      </c>
+      <c r="S108" t="s">
+        <v>71</v>
+      </c>
+      <c r="T108" t="s">
+        <v>72</v>
+      </c>
+      <c r="U108" t="s">
+        <v>72</v>
+      </c>
+      <c r="V108" t="s">
+        <v>72</v>
+      </c>
+      <c r="W108" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>624</v>
+      </c>
+      <c r="B109" t="s">
+        <v>23</v>
+      </c>
+      <c r="C109" t="s">
+        <v>625</v>
+      </c>
+      <c r="D109">
+        <v>91367</v>
+      </c>
+      <c r="E109" t="s">
+        <v>620</v>
+      </c>
+      <c r="F109" t="s">
+        <v>626</v>
+      </c>
+      <c r="G109" t="s">
+        <v>627</v>
+      </c>
+      <c r="H109" t="s">
+        <v>628</v>
+      </c>
+      <c r="I109" t="s">
+        <v>38</v>
+      </c>
+      <c r="J109" t="s">
+        <v>39</v>
+      </c>
+      <c r="K109" t="s">
+        <v>47</v>
+      </c>
+      <c r="L109" t="s">
+        <v>40</v>
+      </c>
+      <c r="M109" t="s">
+        <v>41</v>
+      </c>
+      <c r="N109" t="s">
+        <v>30</v>
+      </c>
+      <c r="O109" t="s">
+        <v>29</v>
+      </c>
+      <c r="P109" t="s">
         <v>629</v>
       </c>
-      <c r="Q108" t="s">
+      <c r="Q109" t="s">
         <v>629</v>
       </c>
-      <c r="R108" t="s">
+      <c r="R109" t="s">
         <v>629</v>
       </c>
-      <c r="S108" t="s">
+      <c r="S109" t="s">
         <v>629</v>
       </c>
-      <c r="T108" t="s">
+      <c r="T109" t="s">
         <v>629</v>
       </c>
-      <c r="U108" t="s">
+      <c r="U109" t="s">
         <v>630</v>
       </c>
-      <c r="V108" t="s">
-        <v>29</v>
-      </c>
-      <c r="W108" t="s">
+      <c r="V109" t="s">
+        <v>29</v>
+      </c>
+      <c r="W109" t="s">
         <v>27</v>
       </c>
     </row>
@@ -10292,16 +10375,17 @@
     <hyperlink ref="H82" r:id="rId3" xr:uid="{AD9CFEB0-515E-47DE-A619-8A0566327566}"/>
     <hyperlink ref="G68" r:id="rId4" xr:uid="{C5402745-E279-4144-A7EA-01FCE7A4E404}"/>
     <hyperlink ref="H68" r:id="rId5" xr:uid="{679F818E-03B4-4BF2-B47A-7E4540C537AF}"/>
-    <hyperlink ref="H103" r:id="rId6" xr:uid="{64B05FEF-865E-4E04-B288-9B0F0E91EB19}"/>
-    <hyperlink ref="G103" r:id="rId7" xr:uid="{1C619C93-40F6-455D-B3C4-D8F5DA0E79E2}"/>
+    <hyperlink ref="H104" r:id="rId6" xr:uid="{64B05FEF-865E-4E04-B288-9B0F0E91EB19}"/>
+    <hyperlink ref="G104" r:id="rId7" xr:uid="{1C619C93-40F6-455D-B3C4-D8F5DA0E79E2}"/>
     <hyperlink ref="H66" r:id="rId8" xr:uid="{811F14D2-8625-407A-A363-4868792D85E3}"/>
     <hyperlink ref="G73" r:id="rId9" xr:uid="{91676D4A-98DC-43A6-8746-157BFB405308}"/>
     <hyperlink ref="H73" r:id="rId10" xr:uid="{03594D0E-5B3F-4FCC-9030-CF67D477ED14}"/>
     <hyperlink ref="H79" r:id="rId11" xr:uid="{9348353F-C4D8-4830-99C4-699BA05B7D2C}"/>
+    <hyperlink ref="H88" r:id="rId12" xr:uid="{A1EF2249-01F0-405D-A76D-A7FF2945CDEA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
email adresse for saloniki added
</commit_message>
<xml_diff>
--- a/cfg/pubfinder_list_NLA.xlsx
+++ b/cfg/pubfinder_list_NLA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_dev\pubfinder_V2\cfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61E5679-4599-43BF-8A88-FCC1FC100A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81CB50A-8F21-4D6F-8501-16E5F6A8B946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{75E81789-C525-4005-96BA-B080353C5F6C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3140" uniqueCount="900">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3145" uniqueCount="901">
   <si>
     <t>Name</t>
   </si>
@@ -2776,6 +2776,9 @@
   </si>
   <si>
     <t>11:00 - 21:30</t>
+  </si>
+  <si>
+    <t>info@grillsaloniki.de</t>
   </si>
 </sst>
 </file>
@@ -3374,8 +3377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F2D7F2-8E23-4C59-B8E8-2949683E6C83}">
   <dimension ref="A1:W147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J40" workbookViewId="0">
-      <selection activeCell="U61" sqref="U61"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7392,6 +7395,9 @@
       <c r="F59" s="2" t="s">
         <v>897</v>
       </c>
+      <c r="G59" s="5" t="s">
+        <v>900</v>
+      </c>
       <c r="H59" s="5" t="s">
         <v>898</v>
       </c>
@@ -13580,11 +13586,12 @@
     <hyperlink ref="H78" r:id="rId21" xr:uid="{55B52E1D-4796-453B-B506-B34A9190D63C}"/>
     <hyperlink ref="H84" r:id="rId22" xr:uid="{D972C143-2111-43B8-8407-AB8CADDF24DF}"/>
     <hyperlink ref="H59" r:id="rId23" xr:uid="{140A89BF-6CB9-4679-AA18-7CA2D32B1C8A}"/>
+    <hyperlink ref="G59" r:id="rId24" xr:uid="{CEA71EAA-2C78-4865-9233-A951E23256B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId24"/>
+  <drawing r:id="rId25"/>
   <tableParts count="1">
-    <tablePart r:id="rId25"/>
+    <tablePart r:id="rId26"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>